<commit_message>
Updated sprint 1 excel sheet with hours
</commit_message>
<xml_diff>
--- a/Sprint_Planning_Document_v2_group.xlsx
+++ b/Sprint_Planning_Document_v2_group.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlenz\OneDrive\Desktop\School_Git\CS491\Team Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ctugroup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECF1856-FB94-40AA-BEAA-C1671D3C0DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC976712-F6E9-4FDE-8CFA-46E7884795DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="De La Cruz, Anthony - Personal View" guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
+    <customWorkbookView name="Sam Burke - Personal View" guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1440" windowHeight="741" activeSheetId="2"/>
     <customWorkbookView name="Anders Pedersen - Personal View" guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="2"/>
-    <customWorkbookView name="Sam Burke - Personal View" guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1440" windowHeight="741" activeSheetId="2"/>
-    <customWorkbookView name="De La Cruz, Anthony - Personal View" guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="126">
   <si>
     <t>What is this?</t>
   </si>
@@ -252,24 +252,6 @@
     <t>Must have types of credit card options for customer to choose from, pay in store option for customers to send to the order in ahead of time and pay during pick-up</t>
   </si>
   <si>
-    <t>Cancel/Change Order</t>
-  </si>
-  <si>
-    <t>Includes option for customer to cancel/change order already placed</t>
-  </si>
-  <si>
-    <t>Must have canceling/change order option for customer, details of how long the customer is able to cancel/change the order before it is too late, description box for customer to enter in reasoning for cancelation to change</t>
-  </si>
-  <si>
-    <t>Order Updates</t>
-  </si>
-  <si>
-    <t>Includes customer's order and time of pick-up</t>
-  </si>
-  <si>
-    <t>Must have avaliable updates to customer of when the pizza is currently being made and when it is ready for pick-up</t>
-  </si>
-  <si>
     <t>User Registration</t>
   </si>
   <si>
@@ -336,15 +318,6 @@
     <t>Must store all menu items, inventory totals, and user accounts. Passwords must be stored encrypted</t>
   </si>
   <si>
-    <t>Reviews</t>
-  </si>
-  <si>
-    <t>Includes past/current customer feedback and experiences</t>
-  </si>
-  <si>
-    <t>Must include customer's name, feedback the customer gave for the pizzeria, star ratings options</t>
-  </si>
-  <si>
     <t>MTG</t>
   </si>
   <si>
@@ -357,12 +330,6 @@
     <t>Welcome Page (Create pizzeria logo)</t>
   </si>
   <si>
-    <t>Welcome Page (Create promotion post)</t>
-  </si>
-  <si>
-    <t>Welcome Page (Create discount post)</t>
-  </si>
-  <si>
     <t>User registration        - Create registration form UI</t>
   </si>
   <si>
@@ -378,9 +345,6 @@
     <t>Scrum Master and Developer Team</t>
   </si>
   <si>
-    <t>Reviews (Create a review tab or link at the bottom of the welcom page)</t>
-  </si>
-  <si>
     <t>Contact Info (Create tab/link on buttom of page next to Reviews for easy access)</t>
   </si>
   <si>
@@ -411,12 +375,6 @@
     <t>Payment Page (Create selection of payment option)</t>
   </si>
   <si>
-    <t>Order Updates Page (Create a separate page for customer's to keep track of when their order is ready for pick-up including time, day, transaction, order list, etc. )</t>
-  </si>
-  <si>
-    <t>Cancel/Change Order Button (Create a button that allows customers to edit their order or cancel it)</t>
-  </si>
-  <si>
     <t>Create database for web site</t>
   </si>
   <si>
@@ -490,6 +448,9 @@
   </si>
   <si>
     <t>Product Owner and Developer Team</t>
+  </si>
+  <si>
+    <t>Welcome Page (Create landing page)</t>
   </si>
 </sst>
 </file>
@@ -1835,27 +1796,27 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$F$40:$S$40</c:f>
+              <c:f>'Sprint 1'!$F$36:$S$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>#N/A</c:v>
+                  <c:v>47.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>#N/A</c:v>
+                  <c:v>46.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>#N/A</c:v>
+                  <c:v>45.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>#N/A</c:v>
+                  <c:v>43.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>#N/A</c:v>
+                  <c:v>40.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>#N/A</c:v>
+                  <c:v>39.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -1924,7 +1885,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1'!$F$41:$S$41</c:f>
+              <c:f>'Sprint 1'!$F$37:$S$37</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2903,13 +2864,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2984,10 +2945,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A10:G21" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11">
-  <autoFilter ref="A10:G21" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:F20">
-    <sortCondition ref="F10:F20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A10:G18" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11">
+  <autoFilter ref="A10:G18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:F18">
+    <sortCondition ref="F10:F18"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name=" Story ID" dataDxfId="10"/>
@@ -3460,8 +3421,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" topLeftCell="A7">
-      <selection activeCell="B12" sqref="B12"/>
+    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}">
+      <selection activeCell="B15" sqref="B15"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
@@ -3472,8 +3433,8 @@
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}">
-      <selection activeCell="B15" sqref="B15"/>
+    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" topLeftCell="A7">
+      <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
@@ -3493,10 +3454,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:EC30"/>
+  <dimension ref="A2:EC27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3749,13 +3710,13 @@
         <v>2</v>
       </c>
       <c r="B12" s="48" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D12" s="48" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E12" s="48">
         <v>1</v>
@@ -3764,7 +3725,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="48" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H12" s="57"/>
       <c r="I12" s="57"/>
@@ -3894,22 +3855,22 @@
       <c r="EC12" s="57"/>
     </row>
     <row r="13" spans="1:133" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="48">
-        <v>3</v>
-      </c>
-      <c r="B13" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" s="48">
+      <c r="A13" s="59">
+        <v>4</v>
+      </c>
+      <c r="B13" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="59">
         <v>2</v>
       </c>
-      <c r="F13" s="48">
+      <c r="F13" s="59">
         <v>1</v>
       </c>
       <c r="G13" s="48" t="s">
@@ -4043,26 +4004,26 @@
       <c r="EC13" s="57"/>
     </row>
     <row r="14" spans="1:133" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="59">
-        <v>4</v>
-      </c>
-      <c r="B14" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="59" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="59" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="59">
-        <v>2</v>
-      </c>
-      <c r="F14" s="59">
+      <c r="A14" s="48">
+        <v>5</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="48">
         <v>1</v>
       </c>
+      <c r="F14" s="48">
+        <v>1</v>
+      </c>
       <c r="G14" s="48" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H14" s="57"/>
       <c r="I14" s="57"/>
@@ -4192,17 +4153,17 @@
       <c r="EC14" s="57"/>
     </row>
     <row r="15" spans="1:133" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="48">
-        <v>5</v>
-      </c>
-      <c r="B15" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="48" t="s">
-        <v>43</v>
+      <c r="A15" s="58">
+        <v>6</v>
+      </c>
+      <c r="B15" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="58" t="s">
+        <v>47</v>
       </c>
       <c r="D15" s="48" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E15" s="48">
         <v>1</v>
@@ -4211,7 +4172,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="48" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="H15" s="57"/>
       <c r="I15" s="57"/>
@@ -4341,17 +4302,17 @@
       <c r="EC15" s="57"/>
     </row>
     <row r="16" spans="1:133" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="58">
-        <v>6</v>
-      </c>
-      <c r="B16" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="58" t="s">
-        <v>47</v>
+      <c r="A16" s="48">
+        <v>7</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>51</v>
       </c>
       <c r="D16" s="48" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E16" s="48">
         <v>1</v>
@@ -4360,7 +4321,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="48" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H16" s="57"/>
       <c r="I16" s="57"/>
@@ -4491,16 +4452,16 @@
     </row>
     <row r="17" spans="1:133" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="48">
-        <v>7</v>
-      </c>
-      <c r="B17" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="48" t="s">
-        <v>51</v>
+        <v>8</v>
+      </c>
+      <c r="B17" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="58" t="s">
+        <v>54</v>
       </c>
       <c r="D17" s="48" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E17" s="48">
         <v>1</v>
@@ -4509,7 +4470,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="48" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="H17" s="57"/>
       <c r="I17" s="57"/>
@@ -4640,16 +4601,16 @@
     </row>
     <row r="18" spans="1:133" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="48">
-        <v>8</v>
-      </c>
-      <c r="B18" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="58" t="s">
-        <v>54</v>
+        <v>9</v>
+      </c>
+      <c r="B18" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="48" t="s">
+        <v>57</v>
       </c>
       <c r="D18" s="48" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E18" s="48">
         <v>1</v>
@@ -4789,16 +4750,16 @@
     </row>
     <row r="19" spans="1:133" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="48">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B19" s="48" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="D19" s="48" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="E19" s="48">
         <v>1</v>
@@ -4807,7 +4768,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="48" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="H19" s="57"/>
       <c r="I19" s="57"/>
@@ -4938,25 +4899,25 @@
     </row>
     <row r="20" spans="1:133" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="48">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B20" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="48">
+        <v>2</v>
+      </c>
+      <c r="F20" s="48">
+        <v>2</v>
+      </c>
+      <c r="G20" s="48" t="s">
         <v>62</v>
-      </c>
-      <c r="C20" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="48">
-        <v>1</v>
-      </c>
-      <c r="F20" s="48">
-        <v>1</v>
-      </c>
-      <c r="G20" s="48" t="s">
-        <v>49</v>
       </c>
       <c r="H20" s="57"/>
       <c r="I20" s="57"/>
@@ -5087,25 +5048,25 @@
     </row>
     <row r="21" spans="1:133" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="48">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B21" s="48" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="E21" s="48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" s="48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G21" s="48" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="H21" s="57"/>
       <c r="I21" s="57"/>
@@ -5236,25 +5197,25 @@
     </row>
     <row r="22" spans="1:133" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="48">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B22" s="48" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="D22" s="48" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="E22" s="48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" s="48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G22" s="48" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="H22" s="57"/>
       <c r="I22" s="57"/>
@@ -5385,16 +5346,16 @@
     </row>
     <row r="23" spans="1:133" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="48">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B23" s="48" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="D23" s="48" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E23" s="48">
         <v>2</v>
@@ -5403,7 +5364,7 @@
         <v>2</v>
       </c>
       <c r="G23" s="48" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="H23" s="57"/>
       <c r="I23" s="57"/>
@@ -5532,478 +5493,31 @@
       <c r="EB23" s="57"/>
       <c r="EC23" s="57"/>
     </row>
-    <row r="24" spans="1:133" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="48">
-        <v>14</v>
-      </c>
-      <c r="B24" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="E24" s="48">
-        <v>2</v>
-      </c>
-      <c r="F24" s="48">
-        <v>2</v>
-      </c>
-      <c r="G24" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="H24" s="57"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="57"/>
-      <c r="M24" s="57"/>
-      <c r="N24" s="57"/>
-      <c r="O24" s="57"/>
-      <c r="P24" s="57"/>
-      <c r="Q24" s="57"/>
-      <c r="R24" s="57"/>
-      <c r="S24" s="57"/>
-      <c r="T24" s="57"/>
-      <c r="U24" s="57"/>
-      <c r="V24" s="57"/>
-      <c r="W24" s="57"/>
-      <c r="X24" s="57"/>
-      <c r="Y24" s="57"/>
-      <c r="Z24" s="57"/>
-      <c r="AA24" s="57"/>
-      <c r="AB24" s="57"/>
-      <c r="AC24" s="57"/>
-      <c r="AD24" s="57"/>
-      <c r="AE24" s="57"/>
-      <c r="AF24" s="57"/>
-      <c r="AG24" s="57"/>
-      <c r="AH24" s="57"/>
-      <c r="AI24" s="57"/>
-      <c r="AJ24" s="57"/>
-      <c r="AK24" s="57"/>
-      <c r="AL24" s="57"/>
-      <c r="AM24" s="57"/>
-      <c r="AN24" s="57"/>
-      <c r="AO24" s="57"/>
-      <c r="AP24" s="57"/>
-      <c r="AQ24" s="57"/>
-      <c r="AR24" s="57"/>
-      <c r="AS24" s="57"/>
-      <c r="AT24" s="57"/>
-      <c r="AU24" s="57"/>
-      <c r="AV24" s="57"/>
-      <c r="AW24" s="57"/>
-      <c r="AX24" s="57"/>
-      <c r="AY24" s="57"/>
-      <c r="AZ24" s="57"/>
-      <c r="BA24" s="57"/>
-      <c r="BB24" s="57"/>
-      <c r="BC24" s="57"/>
-      <c r="BD24" s="57"/>
-      <c r="BE24" s="57"/>
-      <c r="BF24" s="57"/>
-      <c r="BG24" s="57"/>
-      <c r="BH24" s="57"/>
-      <c r="BI24" s="57"/>
-      <c r="BJ24" s="57"/>
-      <c r="BK24" s="57"/>
-      <c r="BL24" s="57"/>
-      <c r="BM24" s="57"/>
-      <c r="BN24" s="57"/>
-      <c r="BO24" s="57"/>
-      <c r="BP24" s="57"/>
-      <c r="BQ24" s="57"/>
-      <c r="BR24" s="57"/>
-      <c r="BS24" s="57"/>
-      <c r="BT24" s="57"/>
-      <c r="BU24" s="57"/>
-      <c r="BV24" s="57"/>
-      <c r="BW24" s="57"/>
-      <c r="BX24" s="57"/>
-      <c r="BY24" s="57"/>
-      <c r="BZ24" s="57"/>
-      <c r="CA24" s="57"/>
-      <c r="CB24" s="57"/>
-      <c r="CC24" s="57"/>
-      <c r="CD24" s="57"/>
-      <c r="CE24" s="57"/>
-      <c r="CF24" s="57"/>
-      <c r="CG24" s="57"/>
-      <c r="CH24" s="57"/>
-      <c r="CI24" s="57"/>
-      <c r="CJ24" s="57"/>
-      <c r="CK24" s="57"/>
-      <c r="CL24" s="57"/>
-      <c r="CM24" s="57"/>
-      <c r="CN24" s="57"/>
-      <c r="CO24" s="57"/>
-      <c r="CP24" s="57"/>
-      <c r="CQ24" s="57"/>
-      <c r="CR24" s="57"/>
-      <c r="CS24" s="57"/>
-      <c r="CT24" s="57"/>
-      <c r="CU24" s="57"/>
-      <c r="CV24" s="57"/>
-      <c r="CW24" s="57"/>
-      <c r="CX24" s="57"/>
-      <c r="CY24" s="57"/>
-      <c r="CZ24" s="57"/>
-      <c r="DA24" s="57"/>
-      <c r="DB24" s="57"/>
-      <c r="DC24" s="57"/>
-      <c r="DD24" s="57"/>
-      <c r="DE24" s="57"/>
-      <c r="DF24" s="57"/>
-      <c r="DG24" s="57"/>
-      <c r="DH24" s="57"/>
-      <c r="DI24" s="57"/>
-      <c r="DJ24" s="57"/>
-      <c r="DK24" s="57"/>
-      <c r="DL24" s="57"/>
-      <c r="DM24" s="57"/>
-      <c r="DN24" s="57"/>
-      <c r="DO24" s="57"/>
-      <c r="DP24" s="57"/>
-      <c r="DQ24" s="57"/>
-      <c r="DR24" s="57"/>
-      <c r="DS24" s="57"/>
-      <c r="DT24" s="57"/>
-      <c r="DU24" s="57"/>
-      <c r="DV24" s="57"/>
-      <c r="DW24" s="57"/>
-      <c r="DX24" s="57"/>
-      <c r="DY24" s="57"/>
-      <c r="DZ24" s="57"/>
-      <c r="EA24" s="57"/>
-      <c r="EB24" s="57"/>
-      <c r="EC24" s="57"/>
-    </row>
-    <row r="25" spans="1:133" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="48">
-        <v>15</v>
-      </c>
-      <c r="B25" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" s="48">
-        <v>2</v>
-      </c>
-      <c r="F25" s="48">
-        <v>2</v>
-      </c>
-      <c r="G25" s="48" t="s">
-        <v>45</v>
-      </c>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="57"/>
-      <c r="L25" s="57"/>
-      <c r="M25" s="57"/>
-      <c r="N25" s="57"/>
-      <c r="O25" s="57"/>
-      <c r="P25" s="57"/>
-      <c r="Q25" s="57"/>
-      <c r="R25" s="57"/>
-      <c r="S25" s="57"/>
-      <c r="T25" s="57"/>
-      <c r="U25" s="57"/>
-      <c r="V25" s="57"/>
-      <c r="W25" s="57"/>
-      <c r="X25" s="57"/>
-      <c r="Y25" s="57"/>
-      <c r="Z25" s="57"/>
-      <c r="AA25" s="57"/>
-      <c r="AB25" s="57"/>
-      <c r="AC25" s="57"/>
-      <c r="AD25" s="57"/>
-      <c r="AE25" s="57"/>
-      <c r="AF25" s="57"/>
-      <c r="AG25" s="57"/>
-      <c r="AH25" s="57"/>
-      <c r="AI25" s="57"/>
-      <c r="AJ25" s="57"/>
-      <c r="AK25" s="57"/>
-      <c r="AL25" s="57"/>
-      <c r="AM25" s="57"/>
-      <c r="AN25" s="57"/>
-      <c r="AO25" s="57"/>
-      <c r="AP25" s="57"/>
-      <c r="AQ25" s="57"/>
-      <c r="AR25" s="57"/>
-      <c r="AS25" s="57"/>
-      <c r="AT25" s="57"/>
-      <c r="AU25" s="57"/>
-      <c r="AV25" s="57"/>
-      <c r="AW25" s="57"/>
-      <c r="AX25" s="57"/>
-      <c r="AY25" s="57"/>
-      <c r="AZ25" s="57"/>
-      <c r="BA25" s="57"/>
-      <c r="BB25" s="57"/>
-      <c r="BC25" s="57"/>
-      <c r="BD25" s="57"/>
-      <c r="BE25" s="57"/>
-      <c r="BF25" s="57"/>
-      <c r="BG25" s="57"/>
-      <c r="BH25" s="57"/>
-      <c r="BI25" s="57"/>
-      <c r="BJ25" s="57"/>
-      <c r="BK25" s="57"/>
-      <c r="BL25" s="57"/>
-      <c r="BM25" s="57"/>
-      <c r="BN25" s="57"/>
-      <c r="BO25" s="57"/>
-      <c r="BP25" s="57"/>
-      <c r="BQ25" s="57"/>
-      <c r="BR25" s="57"/>
-      <c r="BS25" s="57"/>
-      <c r="BT25" s="57"/>
-      <c r="BU25" s="57"/>
-      <c r="BV25" s="57"/>
-      <c r="BW25" s="57"/>
-      <c r="BX25" s="57"/>
-      <c r="BY25" s="57"/>
-      <c r="BZ25" s="57"/>
-      <c r="CA25" s="57"/>
-      <c r="CB25" s="57"/>
-      <c r="CC25" s="57"/>
-      <c r="CD25" s="57"/>
-      <c r="CE25" s="57"/>
-      <c r="CF25" s="57"/>
-      <c r="CG25" s="57"/>
-      <c r="CH25" s="57"/>
-      <c r="CI25" s="57"/>
-      <c r="CJ25" s="57"/>
-      <c r="CK25" s="57"/>
-      <c r="CL25" s="57"/>
-      <c r="CM25" s="57"/>
-      <c r="CN25" s="57"/>
-      <c r="CO25" s="57"/>
-      <c r="CP25" s="57"/>
-      <c r="CQ25" s="57"/>
-      <c r="CR25" s="57"/>
-      <c r="CS25" s="57"/>
-      <c r="CT25" s="57"/>
-      <c r="CU25" s="57"/>
-      <c r="CV25" s="57"/>
-      <c r="CW25" s="57"/>
-      <c r="CX25" s="57"/>
-      <c r="CY25" s="57"/>
-      <c r="CZ25" s="57"/>
-      <c r="DA25" s="57"/>
-      <c r="DB25" s="57"/>
-      <c r="DC25" s="57"/>
-      <c r="DD25" s="57"/>
-      <c r="DE25" s="57"/>
-      <c r="DF25" s="57"/>
-      <c r="DG25" s="57"/>
-      <c r="DH25" s="57"/>
-      <c r="DI25" s="57"/>
-      <c r="DJ25" s="57"/>
-      <c r="DK25" s="57"/>
-      <c r="DL25" s="57"/>
-      <c r="DM25" s="57"/>
-      <c r="DN25" s="57"/>
-      <c r="DO25" s="57"/>
-      <c r="DP25" s="57"/>
-      <c r="DQ25" s="57"/>
-      <c r="DR25" s="57"/>
-      <c r="DS25" s="57"/>
-      <c r="DT25" s="57"/>
-      <c r="DU25" s="57"/>
-      <c r="DV25" s="57"/>
-      <c r="DW25" s="57"/>
-      <c r="DX25" s="57"/>
-      <c r="DY25" s="57"/>
-      <c r="DZ25" s="57"/>
-      <c r="EA25" s="57"/>
-      <c r="EB25" s="57"/>
-      <c r="EC25" s="57"/>
-    </row>
-    <row r="26" spans="1:133" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="48">
-        <v>16</v>
-      </c>
-      <c r="B26" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" s="48" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="48" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" s="48">
-        <v>2</v>
-      </c>
-      <c r="F26" s="48">
-        <v>2</v>
-      </c>
-      <c r="G26" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="H26" s="57"/>
-      <c r="I26" s="57"/>
-      <c r="J26" s="57"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="57"/>
-      <c r="M26" s="57"/>
-      <c r="N26" s="57"/>
-      <c r="O26" s="57"/>
-      <c r="P26" s="57"/>
-      <c r="Q26" s="57"/>
-      <c r="R26" s="57"/>
-      <c r="S26" s="57"/>
-      <c r="T26" s="57"/>
-      <c r="U26" s="57"/>
-      <c r="V26" s="57"/>
-      <c r="W26" s="57"/>
-      <c r="X26" s="57"/>
-      <c r="Y26" s="57"/>
-      <c r="Z26" s="57"/>
-      <c r="AA26" s="57"/>
-      <c r="AB26" s="57"/>
-      <c r="AC26" s="57"/>
-      <c r="AD26" s="57"/>
-      <c r="AE26" s="57"/>
-      <c r="AF26" s="57"/>
-      <c r="AG26" s="57"/>
-      <c r="AH26" s="57"/>
-      <c r="AI26" s="57"/>
-      <c r="AJ26" s="57"/>
-      <c r="AK26" s="57"/>
-      <c r="AL26" s="57"/>
-      <c r="AM26" s="57"/>
-      <c r="AN26" s="57"/>
-      <c r="AO26" s="57"/>
-      <c r="AP26" s="57"/>
-      <c r="AQ26" s="57"/>
-      <c r="AR26" s="57"/>
-      <c r="AS26" s="57"/>
-      <c r="AT26" s="57"/>
-      <c r="AU26" s="57"/>
-      <c r="AV26" s="57"/>
-      <c r="AW26" s="57"/>
-      <c r="AX26" s="57"/>
-      <c r="AY26" s="57"/>
-      <c r="AZ26" s="57"/>
-      <c r="BA26" s="57"/>
-      <c r="BB26" s="57"/>
-      <c r="BC26" s="57"/>
-      <c r="BD26" s="57"/>
-      <c r="BE26" s="57"/>
-      <c r="BF26" s="57"/>
-      <c r="BG26" s="57"/>
-      <c r="BH26" s="57"/>
-      <c r="BI26" s="57"/>
-      <c r="BJ26" s="57"/>
-      <c r="BK26" s="57"/>
-      <c r="BL26" s="57"/>
-      <c r="BM26" s="57"/>
-      <c r="BN26" s="57"/>
-      <c r="BO26" s="57"/>
-      <c r="BP26" s="57"/>
-      <c r="BQ26" s="57"/>
-      <c r="BR26" s="57"/>
-      <c r="BS26" s="57"/>
-      <c r="BT26" s="57"/>
-      <c r="BU26" s="57"/>
-      <c r="BV26" s="57"/>
-      <c r="BW26" s="57"/>
-      <c r="BX26" s="57"/>
-      <c r="BY26" s="57"/>
-      <c r="BZ26" s="57"/>
-      <c r="CA26" s="57"/>
-      <c r="CB26" s="57"/>
-      <c r="CC26" s="57"/>
-      <c r="CD26" s="57"/>
-      <c r="CE26" s="57"/>
-      <c r="CF26" s="57"/>
-      <c r="CG26" s="57"/>
-      <c r="CH26" s="57"/>
-      <c r="CI26" s="57"/>
-      <c r="CJ26" s="57"/>
-      <c r="CK26" s="57"/>
-      <c r="CL26" s="57"/>
-      <c r="CM26" s="57"/>
-      <c r="CN26" s="57"/>
-      <c r="CO26" s="57"/>
-      <c r="CP26" s="57"/>
-      <c r="CQ26" s="57"/>
-      <c r="CR26" s="57"/>
-      <c r="CS26" s="57"/>
-      <c r="CT26" s="57"/>
-      <c r="CU26" s="57"/>
-      <c r="CV26" s="57"/>
-      <c r="CW26" s="57"/>
-      <c r="CX26" s="57"/>
-      <c r="CY26" s="57"/>
-      <c r="CZ26" s="57"/>
-      <c r="DA26" s="57"/>
-      <c r="DB26" s="57"/>
-      <c r="DC26" s="57"/>
-      <c r="DD26" s="57"/>
-      <c r="DE26" s="57"/>
-      <c r="DF26" s="57"/>
-      <c r="DG26" s="57"/>
-      <c r="DH26" s="57"/>
-      <c r="DI26" s="57"/>
-      <c r="DJ26" s="57"/>
-      <c r="DK26" s="57"/>
-      <c r="DL26" s="57"/>
-      <c r="DM26" s="57"/>
-      <c r="DN26" s="57"/>
-      <c r="DO26" s="57"/>
-      <c r="DP26" s="57"/>
-      <c r="DQ26" s="57"/>
-      <c r="DR26" s="57"/>
-      <c r="DS26" s="57"/>
-      <c r="DT26" s="57"/>
-      <c r="DU26" s="57"/>
-      <c r="DV26" s="57"/>
-      <c r="DW26" s="57"/>
-      <c r="DX26" s="57"/>
-      <c r="DY26" s="57"/>
-      <c r="DZ26" s="57"/>
-      <c r="EA26" s="57"/>
-      <c r="EB26" s="57"/>
-      <c r="EC26" s="57"/>
-    </row>
-    <row r="28" spans="1:133" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:133" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:133" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:133" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:133" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:133" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" showAutoFilter="1">
-      <selection activeCell="B43" sqref="B43"/>
+    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" showAutoFilter="1">
+      <selection activeCell="B7" sqref="B7"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{2D290C7E-0FF1-4575-92D0-3CC184BED031}"/>
+      <autoFilter ref="B1:F1" xr:uid="{AC3AA21D-558C-42B9-AFD3-DEC2AA8F64B5}"/>
     </customSheetView>
     <customSheetView guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" scale="150" showAutoFilter="1" topLeftCell="B36">
       <selection activeCell="C41" sqref="C41"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{D13EB277-6D92-4E20-A4FC-6AB91B2EA786}"/>
+      <autoFilter ref="B1:F1" xr:uid="{7F2F6814-86B1-4863-AF2A-10461B55DF12}"/>
     </customSheetView>
-    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" showAutoFilter="1">
-      <selection activeCell="B7" sqref="B7"/>
+    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" showAutoFilter="1">
+      <selection activeCell="B43" sqref="B43"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{66B21AF5-5C63-4D3B-8B9E-906D7E602E33}"/>
+      <autoFilter ref="B1:F1" xr:uid="{FD189D20-B022-4CD5-9675-39B0E7B2D990}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -6021,10 +5535,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31AAAAEB-B5F0-468C-BFDD-E9B5D3EFF0AD}">
-  <dimension ref="A2:S44"/>
+  <dimension ref="A2:S40"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6236,25 +5750,29 @@
     </row>
     <row r="11" spans="1:19" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D11" s="61" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E11" s="25">
         <v>1</v>
       </c>
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
+      <c r="H11" s="29">
+        <v>1.5</v>
+      </c>
       <c r="I11" s="29"/>
-      <c r="J11" s="27"/>
+      <c r="J11" s="27">
+        <v>0.5</v>
+      </c>
       <c r="K11" s="27"/>
       <c r="L11" s="27"/>
       <c r="M11" s="29"/>
@@ -6273,7 +5791,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D12" s="61" t="s">
         <v>14</v>
@@ -6281,7 +5799,9 @@
       <c r="E12" s="25">
         <v>2</v>
       </c>
-      <c r="F12" s="29"/>
+      <c r="F12" s="29">
+        <v>0.75</v>
+      </c>
       <c r="G12" s="29"/>
       <c r="H12" s="29"/>
       <c r="I12" s="29"/>
@@ -6296,7 +5816,7 @@
       <c r="R12" s="27"/>
       <c r="S12" s="27"/>
     </row>
-    <row r="13" spans="1:19" s="30" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13" s="26">
         <v>1.2</v>
       </c>
@@ -6304,18 +5824,22 @@
         <v>1</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="D13" s="61" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E13" s="25">
         <v>2</v>
       </c>
       <c r="F13" s="29"/>
-      <c r="G13" s="27"/>
+      <c r="G13" s="27">
+        <v>0.5</v>
+      </c>
       <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
+      <c r="I13" s="27">
+        <v>1</v>
+      </c>
       <c r="J13" s="27"/>
       <c r="K13" s="27"/>
       <c r="L13" s="27"/>
@@ -6327,27 +5851,29 @@
       <c r="R13" s="27"/>
       <c r="S13" s="27"/>
     </row>
-    <row r="14" spans="1:19" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" s="30" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="26">
-        <v>1.3</v>
+        <v>2.1</v>
       </c>
       <c r="B14" s="27">
+        <v>2</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="25">
         <v>1</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D14" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="25">
-        <v>2</v>
       </c>
       <c r="F14" s="29"/>
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
+      <c r="J14" s="27">
+        <v>1</v>
+      </c>
       <c r="K14" s="27"/>
       <c r="L14" s="27"/>
       <c r="M14" s="29"/>
@@ -6360,25 +5886,27 @@
     </row>
     <row r="15" spans="1:19" s="30" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="26">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B15" s="27">
         <v>2</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D15" s="61" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E15" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="29"/>
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
+      <c r="J15" s="27">
+        <v>1</v>
+      </c>
       <c r="K15" s="27"/>
       <c r="L15" s="27"/>
       <c r="M15" s="29"/>
@@ -6389,88 +5917,90 @@
       <c r="R15" s="27"/>
       <c r="S15" s="27"/>
     </row>
-    <row r="16" spans="1:19" s="30" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="26">
-        <v>2.2000000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B16" s="27">
         <v>2</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D16" s="61" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E16" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="29"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
       <c r="M16" s="29"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="27"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
     </row>
     <row r="17" spans="1:19" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="26">
-        <v>2.2999999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="B17" s="27">
         <v>2</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="D17" s="61" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="E17" s="25">
         <v>1</v>
       </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-    </row>
-    <row r="18" spans="1:19" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="26">
-        <v>2.4</v>
-      </c>
-      <c r="B18" s="27">
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+    </row>
+    <row r="18" spans="1:19" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="62">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B18" s="63">
+        <v>4</v>
+      </c>
+      <c r="C18" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="65">
         <v>2</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="D18" s="61" t="s">
-        <v>100</v>
-      </c>
-      <c r="E18" s="25">
-        <v>1</v>
       </c>
       <c r="F18" s="29"/>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
+      <c r="I18" s="21">
+        <v>1</v>
+      </c>
       <c r="J18" s="21"/>
       <c r="K18" s="21"/>
       <c r="L18" s="21"/>
@@ -6483,20 +6013,20 @@
       <c r="S18" s="21"/>
     </row>
     <row r="19" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="62">
-        <v>3.1</v>
-      </c>
-      <c r="B19" s="63">
-        <v>3</v>
-      </c>
-      <c r="C19" s="64" t="s">
-        <v>101</v>
+      <c r="A19" s="26">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B19" s="27">
+        <v>5</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>91</v>
       </c>
       <c r="D19" s="61" t="s">
-        <v>138</v>
-      </c>
-      <c r="E19" s="65">
-        <v>3.5</v>
+        <v>45</v>
+      </c>
+      <c r="E19" s="25">
+        <v>1</v>
       </c>
       <c r="F19" s="29"/>
       <c r="G19" s="21"/>
@@ -6513,21 +6043,21 @@
       <c r="R19" s="21"/>
       <c r="S19" s="21"/>
     </row>
-    <row r="20" spans="1:19" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="62">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B20" s="63">
-        <v>4</v>
-      </c>
-      <c r="C20" s="64" t="s">
-        <v>102</v>
+    <row r="20" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="27">
+        <v>5</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>92</v>
       </c>
       <c r="D20" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="65">
-        <v>2</v>
+      <c r="E20" s="25">
+        <v>1</v>
       </c>
       <c r="F20" s="29"/>
       <c r="G20" s="21"/>
@@ -6546,16 +6076,16 @@
     </row>
     <row r="21" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="26">
-        <v>5.0999999999999996</v>
+        <v>5.3</v>
       </c>
       <c r="B21" s="27">
         <v>5</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D21" s="61" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="E21" s="25">
         <v>1</v>
@@ -6576,20 +6106,20 @@
       <c r="S21" s="21"/>
     </row>
     <row r="22" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="26" t="s">
-        <v>117</v>
+      <c r="A22" s="26">
+        <v>6.1</v>
       </c>
       <c r="B22" s="27">
-        <v>5</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>104</v>
+        <v>6</v>
+      </c>
+      <c r="C22" s="64" t="s">
+        <v>94</v>
       </c>
       <c r="D22" s="61" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E22" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="21"/>
@@ -6608,16 +6138,16 @@
     </row>
     <row r="23" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="26">
-        <v>5.3</v>
+        <v>6.2</v>
       </c>
       <c r="B23" s="27">
-        <v>5</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>105</v>
+        <v>6</v>
+      </c>
+      <c r="C23" s="64" t="s">
+        <v>95</v>
       </c>
       <c r="D23" s="61" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E23" s="25">
         <v>1</v>
@@ -6639,16 +6169,16 @@
     </row>
     <row r="24" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="26">
-        <v>6.1</v>
+        <v>6.3</v>
       </c>
       <c r="B24" s="27">
         <v>6</v>
       </c>
       <c r="C24" s="64" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D24" s="61" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E24" s="25">
         <v>2</v>
@@ -6668,18 +6198,18 @@
       <c r="R24" s="21"/>
       <c r="S24" s="21"/>
     </row>
-    <row r="25" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A25" s="26">
-        <v>6.2</v>
+        <v>7.1</v>
       </c>
       <c r="B25" s="27">
-        <v>6</v>
-      </c>
-      <c r="C25" s="64" t="s">
-        <v>107</v>
+        <v>7</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>97</v>
       </c>
       <c r="D25" s="61" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="E25" s="25">
         <v>1</v>
@@ -6699,317 +6229,346 @@
       <c r="R25" s="21"/>
       <c r="S25" s="21"/>
     </row>
-    <row r="26" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="26">
-        <v>6.3</v>
-      </c>
-      <c r="B26" s="27">
-        <v>6</v>
+    <row r="26" spans="1:19" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="62">
+        <v>8.1</v>
+      </c>
+      <c r="B26" s="63">
+        <v>8</v>
       </c>
       <c r="C26" s="64" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D26" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" s="25">
-        <v>2</v>
-      </c>
-      <c r="F26" s="29"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="21"/>
-      <c r="O26" s="21"/>
-      <c r="P26" s="21"/>
-      <c r="Q26" s="21"/>
-      <c r="R26" s="21"/>
-      <c r="S26" s="21"/>
-    </row>
-    <row r="27" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="26">
-        <v>7.1</v>
-      </c>
-      <c r="B27" s="27">
-        <v>7</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>109</v>
+        <v>89</v>
+      </c>
+      <c r="E26" s="65">
+        <v>5</v>
+      </c>
+      <c r="F26" s="66"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="66"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="23"/>
+      <c r="R26" s="23"/>
+      <c r="S26" s="23"/>
+    </row>
+    <row r="27" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="62">
+        <v>9.1</v>
+      </c>
+      <c r="B27" s="63">
+        <v>9</v>
+      </c>
+      <c r="C27" s="64" t="s">
+        <v>99</v>
       </c>
       <c r="D27" s="61" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="25">
+        <v>124</v>
+      </c>
+      <c r="E27" s="65">
+        <v>5</v>
+      </c>
+      <c r="F27" s="66"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="66"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+    </row>
+    <row r="28" spans="1:19" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="27">
+        <v>12.1</v>
+      </c>
+      <c r="B28" s="27">
+        <v>12</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="F28" s="29"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="L28" s="21"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="21"/>
+      <c r="S28" s="21"/>
+    </row>
+    <row r="29" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="27">
+        <v>12.2</v>
+      </c>
+      <c r="B29" s="27">
+        <v>12</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="25">
         <v>1</v>
       </c>
-      <c r="F27" s="29"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="21"/>
-      <c r="O27" s="21"/>
-      <c r="P27" s="21"/>
-      <c r="Q27" s="21"/>
-      <c r="R27" s="21"/>
-      <c r="S27" s="21"/>
-    </row>
-    <row r="28" spans="1:19" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="62">
-        <v>8.1</v>
-      </c>
-      <c r="B28" s="63">
-        <v>8</v>
-      </c>
-      <c r="C28" s="64" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="61" t="s">
-        <v>100</v>
-      </c>
-      <c r="E28" s="65">
-        <v>5</v>
-      </c>
-      <c r="F28" s="66"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="66"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="23"/>
-    </row>
-    <row r="29" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="62">
-        <v>9.1</v>
-      </c>
-      <c r="B29" s="63">
-        <v>9</v>
-      </c>
-      <c r="C29" s="64" t="s">
-        <v>111</v>
-      </c>
-      <c r="D29" s="61" t="s">
-        <v>138</v>
-      </c>
-      <c r="E29" s="65">
-        <v>5</v>
-      </c>
-      <c r="F29" s="66"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="66"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
-    </row>
-    <row r="30" spans="1:19" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="62">
-        <v>10.1</v>
-      </c>
-      <c r="B30" s="63">
-        <v>10</v>
-      </c>
-      <c r="C30" s="64" t="s">
-        <v>112</v>
+      <c r="F29" s="29"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="L29" s="21"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
+    </row>
+    <row r="30" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="27">
+        <v>12.3</v>
+      </c>
+      <c r="B30" s="27">
+        <v>12</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>102</v>
       </c>
       <c r="D30" s="61" t="s">
-        <v>100</v>
-      </c>
-      <c r="E30" s="65">
-        <v>5</v>
-      </c>
-      <c r="F30" s="66"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="66"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="23"/>
-      <c r="Q30" s="23"/>
-      <c r="R30" s="23"/>
-      <c r="S30" s="23"/>
-    </row>
-    <row r="31" spans="1:19" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="62">
-        <v>11.1</v>
-      </c>
-      <c r="B31" s="63">
-        <v>11</v>
-      </c>
-      <c r="C31" s="64" t="s">
-        <v>113</v>
+        <v>13</v>
+      </c>
+      <c r="E30" s="25">
+        <v>1</v>
+      </c>
+      <c r="F30" s="29"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="L30" s="21"/>
+      <c r="M30" s="27"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="21"/>
+    </row>
+    <row r="31" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>104</v>
       </c>
       <c r="D31" s="61" t="s">
-        <v>100</v>
-      </c>
-      <c r="E31" s="65">
-        <v>1.5</v>
-      </c>
-      <c r="F31" s="66"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="23"/>
-      <c r="M31" s="66"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="23"/>
-      <c r="P31" s="23"/>
-      <c r="Q31" s="23"/>
-      <c r="R31" s="23"/>
-      <c r="S31" s="23"/>
-    </row>
-    <row r="32" spans="1:19" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="27">
-        <v>12.1</v>
-      </c>
-      <c r="B32" s="27">
-        <v>12</v>
-      </c>
-      <c r="C32" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="D32" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="25">
-        <v>0.5</v>
-      </c>
-      <c r="F32" s="29"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="21"/>
-      <c r="O32" s="21"/>
-      <c r="P32" s="21"/>
-      <c r="Q32" s="21"/>
-      <c r="R32" s="21"/>
-      <c r="S32" s="21"/>
-    </row>
-    <row r="33" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="27">
-        <v>12.2</v>
-      </c>
-      <c r="B33" s="27">
-        <v>12</v>
-      </c>
-      <c r="C33" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="D33" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="25">
+        <v>49</v>
+      </c>
+      <c r="E31" s="25">
         <v>1</v>
       </c>
-      <c r="F33" s="29"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="27"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="21"/>
-      <c r="P33" s="21"/>
-      <c r="Q33" s="21"/>
-      <c r="R33" s="21"/>
-      <c r="S33" s="21"/>
-    </row>
-    <row r="34" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="27">
-        <v>12.3</v>
-      </c>
-      <c r="B34" s="27">
-        <v>12</v>
-      </c>
-      <c r="C34" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="D34" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="25">
-        <v>1</v>
-      </c>
-      <c r="F34" s="29"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="27"/>
-      <c r="N34" s="21"/>
-      <c r="O34" s="21"/>
-      <c r="P34" s="21"/>
-      <c r="Q34" s="21"/>
-      <c r="R34" s="21"/>
-      <c r="S34" s="21"/>
-    </row>
-    <row r="35" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="B35" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="C35" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="D35" s="61" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="25">
-        <v>1</v>
-      </c>
-      <c r="F35" s="29"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
-      <c r="L35" s="21"/>
-      <c r="M35" s="27"/>
-      <c r="N35" s="21"/>
-      <c r="O35" s="21"/>
-      <c r="P35" s="21"/>
-      <c r="Q35" s="21"/>
-      <c r="R35" s="21"/>
-      <c r="S35" s="21"/>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="F31" s="29"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="27"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+    </row>
+    <row r="34" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+    </row>
+    <row r="35" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+    </row>
+    <row r="36" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C36" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="53"/>
+      <c r="E36" s="79">
+        <f>8*2*E7</f>
+        <v>48</v>
+      </c>
+      <c r="F36" s="8">
+        <f>IF(SUM(F11:F31)&gt;0,E36-SUM(F11:F31),NA())</f>
+        <v>47.25</v>
+      </c>
+      <c r="G36" s="8">
+        <f>IF(SUM(G11:G31)&gt;0,E36-SUM(F11:G31),NA())</f>
+        <v>46.75</v>
+      </c>
+      <c r="H36" s="8">
+        <f>IF(SUM(H11:H31)&gt;0,F36-SUM(G11:H31),NA())</f>
+        <v>45.25</v>
+      </c>
+      <c r="I36" s="8">
+        <f>IF(SUM(I11:I31)&gt;0,E36-SUM(F11:I31),NA())</f>
+        <v>43.25</v>
+      </c>
+      <c r="J36" s="8">
+        <f>IF(SUM(J11:J31)&gt;0,E36-SUM(F11:J31),NA())</f>
+        <v>40.75</v>
+      </c>
+      <c r="K36" s="8">
+        <f>IF(SUM(K11:K31)&gt;0,E36-SUM(F11:K31),NA())</f>
+        <v>39.25</v>
+      </c>
+      <c r="L36" s="8" t="e">
+        <f>IF(SUM(L11:L31)&gt;0,E36-SUM(F11:L31),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M36" s="8" t="e">
+        <f>IF(SUM(M11:M31)&gt;0,L36-SUM(M11:M31),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N36" s="8" t="e">
+        <f>IF(SUM(N11:N31)&gt;0,L36-SUM(M11:N31),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O36" s="8" t="e">
+        <f>IF(SUM(O11:O31)&gt;0,M36-SUM(N11:O31),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P36" s="8" t="e">
+        <f>IF(SUM(P11:P31)&gt;0,L36-SUM(M11:P31),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q36" s="8" t="e">
+        <f>IF(SUM(Q11:Q31)&gt;0,L36-SUM(M11:Q31),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R36" s="8" t="e">
+        <f>IF(SUM(R11:R31)&gt;0,L36-SUM(M11:R31),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S36" s="8" t="e">
+        <f>IF(SUM(S11:S31)&gt;0,L36-SUM(M11:S31),NA())</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="37" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C37" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="54"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="9">
+        <f>E36-(E36/14)</f>
+        <v>44.571428571428569</v>
+      </c>
+      <c r="G37" s="9">
+        <f>F37-(E36/14)</f>
+        <v>41.142857142857139</v>
+      </c>
+      <c r="H37" s="9">
+        <f>G37-(E36/14)</f>
+        <v>37.714285714285708</v>
+      </c>
+      <c r="I37" s="9">
+        <f>H37-(E36/14)</f>
+        <v>34.285714285714278</v>
+      </c>
+      <c r="J37" s="9">
+        <f>I37-(E36/14)</f>
+        <v>30.857142857142851</v>
+      </c>
+      <c r="K37" s="9">
+        <f>J37-(E36/14)</f>
+        <v>27.428571428571423</v>
+      </c>
+      <c r="L37" s="9">
+        <f>K37-(E36/14)</f>
+        <v>23.999999999999996</v>
+      </c>
+      <c r="M37" s="9">
+        <f>L37-(E36/14)</f>
+        <v>20.571428571428569</v>
+      </c>
+      <c r="N37" s="9">
+        <f>M37-(E36/14)</f>
+        <v>17.142857142857142</v>
+      </c>
+      <c r="O37" s="9">
+        <f>N37-(E36/14)</f>
+        <v>13.714285714285714</v>
+      </c>
+      <c r="P37" s="9">
+        <f>O37-(E36/14)</f>
+        <v>10.285714285714285</v>
+      </c>
+      <c r="Q37" s="9">
+        <f>P37-(E36/14)</f>
+        <v>6.8571428571428559</v>
+      </c>
+      <c r="R37" s="9">
+        <f>Q37-(E36/14)</f>
+        <v>3.4285714285714275</v>
+      </c>
+      <c r="S37" s="9">
+        <f>R37-(E36/14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="3:19" x14ac:dyDescent="0.2">
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
@@ -7018,7 +6577,7 @@
       <c r="R38" s="4"/>
       <c r="S38" s="4"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:19" x14ac:dyDescent="0.2">
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
@@ -7027,161 +6586,14 @@
       <c r="R39" s="4"/>
       <c r="S39" s="4"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C40" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D40" s="53"/>
-      <c r="E40" s="79">
-        <f>8*2*E7</f>
-        <v>48</v>
-      </c>
-      <c r="F40" s="8" t="e">
-        <f>IF(SUM(F11:F18)&gt;0,E40-SUM(F11:F18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G40" s="8" t="e">
-        <f>IF(SUM(G11:G18)&gt;0,E40-SUM(F11:G18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H40" s="8" t="e">
-        <f>IF(SUM(H11:H18)&gt;0,F40-SUM(G11:H18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I40" s="8" t="e">
-        <f>IF(SUM(I11:I18)&gt;0,E40-SUM(F11:I18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J40" s="8" t="e">
-        <f>IF(SUM(J11:J18)&gt;0,E40-SUM(F11:J18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K40" s="8" t="e">
-        <f>IF(SUM(K11:K18)&gt;0,E40-SUM(F11:K18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L40" s="8" t="e">
-        <f>IF(SUM(L11:L18)&gt;0,E40-SUM(F11:L18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M40" s="8" t="e">
-        <f>IF(SUM(M11:M18)&gt;0,L40-SUM(M11:M18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N40" s="8" t="e">
-        <f>IF(SUM(N11:N18)&gt;0,L40-SUM(M11:N18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O40" s="8" t="e">
-        <f>IF(SUM(O11:O18)&gt;0,M40-SUM(N11:O18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P40" s="8" t="e">
-        <f>IF(SUM(P11:P18)&gt;0,L40-SUM(M11:P18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q40" s="8" t="e">
-        <f>IF(SUM(Q11:Q18)&gt;0,L40-SUM(M11:Q18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R40" s="8" t="e">
-        <f>IF(SUM(R11:R18)&gt;0,L40-SUM(M11:R18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S40" s="8" t="e">
-        <f>IF(SUM(S11:S18)&gt;0,L40-SUM(M11:S18),NA())</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C41" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D41" s="54"/>
-      <c r="E41" s="80"/>
-      <c r="F41" s="9">
-        <f>E40-(E40/14)</f>
-        <v>44.571428571428569</v>
-      </c>
-      <c r="G41" s="9">
-        <f>F41-(E40/14)</f>
-        <v>41.142857142857139</v>
-      </c>
-      <c r="H41" s="9">
-        <f>G41-(E40/14)</f>
-        <v>37.714285714285708</v>
-      </c>
-      <c r="I41" s="9">
-        <f>H41-(E40/14)</f>
-        <v>34.285714285714278</v>
-      </c>
-      <c r="J41" s="9">
-        <f>I41-(E40/14)</f>
-        <v>30.857142857142851</v>
-      </c>
-      <c r="K41" s="9">
-        <f>J41-(E40/14)</f>
-        <v>27.428571428571423</v>
-      </c>
-      <c r="L41" s="9">
-        <f>K41-(E40/14)</f>
-        <v>23.999999999999996</v>
-      </c>
-      <c r="M41" s="9">
-        <f>L41-(E40/14)</f>
-        <v>20.571428571428569</v>
-      </c>
-      <c r="N41" s="9">
-        <f>M41-(E40/14)</f>
-        <v>17.142857142857142</v>
-      </c>
-      <c r="O41" s="9">
-        <f>N41-(E40/14)</f>
-        <v>13.714285714285714</v>
-      </c>
-      <c r="P41" s="9">
-        <f>O41-(E40/14)</f>
-        <v>10.285714285714285</v>
-      </c>
-      <c r="Q41" s="9">
-        <f>P41-(E40/14)</f>
-        <v>6.8571428571428559</v>
-      </c>
-      <c r="R41" s="9">
-        <f>Q41-(E40/14)</f>
-        <v>3.4285714285714275</v>
-      </c>
-      <c r="S41" s="9">
-        <f>R41-(E40/14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
-      <c r="O42" s="4"/>
-      <c r="P42" s="4"/>
-      <c r="Q42" s="4"/>
-      <c r="R42" s="4"/>
-      <c r="S42" s="4"/>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-      <c r="P43" s="4"/>
-      <c r="Q43" s="4"/>
-      <c r="R43" s="4"/>
-      <c r="S43" s="4"/>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
-      <c r="Q44" s="4"/>
-      <c r="R44" s="4"/>
-      <c r="S44" s="4"/>
+    <row r="40" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="4"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" autoFilter="0"/>
@@ -7191,14 +6603,14 @@
     <mergeCell ref="E4:J4"/>
     <mergeCell ref="F8:L8"/>
     <mergeCell ref="M8:S8"/>
-    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="E36:E37"/>
   </mergeCells>
-  <conditionalFormatting sqref="F40:S40">
+  <conditionalFormatting sqref="F36:S36">
     <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="lessThan">
-      <formula>F41</formula>
+      <formula>F37</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="greaterThan">
-      <formula>F41</formula>
+      <formula>F37</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7211,8 +6623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482CBEFA-189F-463E-82F1-D402C5EC0D1D}">
   <dimension ref="A2:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7424,13 +6836,13 @@
     </row>
     <row r="11" spans="1:19" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="D11" s="61" t="s">
         <v>49</v>
@@ -7461,7 +6873,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="D12" s="61" t="s">
         <v>14</v>
@@ -7492,10 +6904,10 @@
         <v>13</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="D13" s="61" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="E13" s="25">
         <v>1.5</v>
@@ -7523,10 +6935,10 @@
         <v>14</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="D14" s="61" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E14" s="25">
         <v>1</v>
@@ -7554,10 +6966,10 @@
         <v>14</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="D15" s="61" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E15" s="25">
         <v>1</v>
@@ -7585,10 +6997,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="D16" s="61" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E16" s="25">
         <v>1</v>
@@ -7616,7 +7028,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="64" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="D17" s="61" t="s">
         <v>45</v>
@@ -7647,7 +7059,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="64" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="D18" s="61" t="s">
         <v>45</v>
@@ -7678,7 +7090,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D19" s="61" t="s">
         <v>45</v>
@@ -7709,7 +7121,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="64" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="D20" s="61" t="s">
         <v>49</v>
@@ -7740,7 +7152,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="64" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="D21" s="61" t="s">
         <v>49</v>
@@ -7765,13 +7177,13 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="D22" s="61" t="s">
         <v>49</v>
@@ -7796,13 +7208,13 @@
     </row>
     <row r="23" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A23" s="27" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="D23" s="61" t="s">
         <v>49</v>
@@ -7827,13 +7239,13 @@
     </row>
     <row r="24" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A24" s="27" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D24" s="61" t="s">
         <v>49</v>
@@ -7858,13 +7270,13 @@
     </row>
     <row r="25" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A25" s="27" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="D25" s="61" t="s">
         <v>49</v>
@@ -7889,13 +7301,13 @@
     </row>
     <row r="26" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A26" s="27" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="D26" s="61" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Created sprint 1 todo list
</commit_message>
<xml_diff>
--- a/Sprint_Planning_Document_v2_group.xlsx
+++ b/Sprint_Planning_Document_v2_group.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ctugroup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC976712-F6E9-4FDE-8CFA-46E7884795DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBC2DE6-424F-42BE-A9D2-B895D253A952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="125">
   <si>
     <t>What is this?</t>
   </si>
@@ -436,9 +436,6 @@
   </si>
   <si>
     <t>Create logic to use third party API to securely process paymeny</t>
-  </si>
-  <si>
-    <t>Confirm SSL certificate for site</t>
   </si>
   <si>
     <t>Encrypt passwords in database</t>
@@ -2355,7 +2352,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2'!$F$33:$S$33</c:f>
+              <c:f>'Sprint 2'!$F$32:$S$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2444,7 +2441,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2'!$F$34:$S$34</c:f>
+              <c:f>'Sprint 2'!$F$33:$S$33</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="14"/>
@@ -2907,13 +2904,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>790575</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5537,8 +5534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31AAAAEB-B5F0-468C-BFDD-E9B5D3EFF0AD}">
   <dimension ref="A2:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5824,7 +5821,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D13" s="61" t="s">
         <v>62</v>
@@ -6271,7 +6268,7 @@
         <v>99</v>
       </c>
       <c r="D27" s="61" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E27" s="65">
         <v>5</v>
@@ -6621,10 +6618,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482CBEFA-189F-463E-82F1-D402C5EC0D1D}">
-  <dimension ref="A2:S44"/>
+  <dimension ref="A2:S43"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="S33" sqref="S33"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6907,7 +6904,7 @@
         <v>120</v>
       </c>
       <c r="D13" s="61" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E13" s="25">
         <v>1.5</v>
@@ -6929,7 +6926,7 @@
     </row>
     <row r="14" spans="1:19" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A14" s="26">
-        <v>14.1</v>
+        <v>14.2</v>
       </c>
       <c r="B14" s="44">
         <v>14</v>
@@ -6960,7 +6957,7 @@
     </row>
     <row r="15" spans="1:19" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A15" s="26">
-        <v>14.2</v>
+        <v>14.3</v>
       </c>
       <c r="B15" s="44">
         <v>14</v>
@@ -6989,77 +6986,77 @@
       <c r="R15" s="27"/>
       <c r="S15" s="27"/>
     </row>
-    <row r="16" spans="1:19" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="26">
-        <v>14.3</v>
-      </c>
-      <c r="B16" s="44">
-        <v>14</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>123</v>
+        <v>15.1</v>
+      </c>
+      <c r="B16" s="27">
+        <v>15</v>
+      </c>
+      <c r="C16" s="64" t="s">
+        <v>106</v>
       </c>
       <c r="D16" s="61" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="E16" s="25">
         <v>1</v>
       </c>
       <c r="F16" s="29"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
       <c r="M16" s="29"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="27"/>
-    </row>
-    <row r="17" spans="1:19" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="26">
-        <v>15.1</v>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+    </row>
+    <row r="17" spans="1:19" s="30" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="62">
+        <v>15.2</v>
       </c>
       <c r="B17" s="27">
         <v>15</v>
       </c>
       <c r="C17" s="64" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D17" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="25">
-        <v>1</v>
+      <c r="E17" s="65">
+        <v>2</v>
       </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
       <c r="M17" s="29"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="27"/>
+      <c r="S17" s="27"/>
     </row>
     <row r="18" spans="1:19" s="30" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="62">
-        <v>15.2</v>
+        <v>15.3</v>
       </c>
       <c r="B18" s="27">
         <v>15</v>
       </c>
       <c r="C18" s="64" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D18" s="61" t="s">
         <v>45</v>
@@ -7084,50 +7081,50 @@
     </row>
     <row r="19" spans="1:19" s="30" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="62">
-        <v>15.3</v>
-      </c>
-      <c r="B19" s="27">
-        <v>15</v>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="B19" s="63">
+        <v>16</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D19" s="61" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E19" s="65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
       <c r="J19" s="27"/>
       <c r="K19" s="27"/>
       <c r="L19" s="27"/>
       <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="29"/>
+      <c r="N19" s="27"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="27"/>
       <c r="Q19" s="27"/>
       <c r="R19" s="27"/>
       <c r="S19" s="27"/>
     </row>
     <row r="20" spans="1:19" s="30" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="62">
-        <v>16.100000000000001</v>
+        <v>16.2</v>
       </c>
       <c r="B20" s="63">
         <v>16</v>
       </c>
       <c r="C20" s="64" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D20" s="61" t="s">
         <v>49</v>
       </c>
       <c r="E20" s="65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" s="29"/>
       <c r="G20" s="27"/>
@@ -7144,46 +7141,46 @@
       <c r="R20" s="27"/>
       <c r="S20" s="27"/>
     </row>
-    <row r="21" spans="1:19" s="30" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="62">
-        <v>16.2</v>
-      </c>
-      <c r="B21" s="63">
-        <v>16</v>
-      </c>
-      <c r="C21" s="64" t="s">
-        <v>110</v>
+    <row r="21" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>112</v>
       </c>
       <c r="D21" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="65">
+      <c r="E21" s="25">
         <v>2</v>
       </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="27"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
     </row>
     <row r="22" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>82</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D22" s="61" t="s">
         <v>49</v>
@@ -7208,19 +7205,19 @@
     </row>
     <row r="23" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A23" s="27" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>82</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D23" s="61" t="s">
         <v>49</v>
       </c>
       <c r="E23" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" s="29"/>
       <c r="G23" s="21"/>
@@ -7239,13 +7236,13 @@
     </row>
     <row r="24" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A24" s="27" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="B24" s="27" t="s">
         <v>82</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D24" s="61" t="s">
         <v>49</v>
@@ -7276,7 +7273,7 @@
         <v>82</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D25" s="61" t="s">
         <v>49</v>
@@ -7299,22 +7296,12 @@
       <c r="R25" s="21"/>
       <c r="S25" s="21"/>
     </row>
-    <row r="26" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="D26" s="61" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="25">
-        <v>1</v>
-      </c>
+    <row r="26" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="26"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="25"/>
       <c r="F26" s="29"/>
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
@@ -7322,7 +7309,7 @@
       <c r="J26" s="21"/>
       <c r="K26" s="21"/>
       <c r="L26" s="21"/>
-      <c r="M26" s="27"/>
+      <c r="M26" s="29"/>
       <c r="N26" s="21"/>
       <c r="O26" s="21"/>
       <c r="P26" s="21"/>
@@ -7330,26 +7317,26 @@
       <c r="R26" s="21"/>
       <c r="S26" s="21"/>
     </row>
-    <row r="27" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="26"/>
       <c r="B27" s="44"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="67"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="52"/>
       <c r="E27" s="25"/>
       <c r="F27" s="29"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
       <c r="M27" s="29"/>
-      <c r="N27" s="21"/>
-      <c r="O27" s="21"/>
-      <c r="P27" s="21"/>
-      <c r="Q27" s="21"/>
-      <c r="R27" s="21"/>
-      <c r="S27" s="21"/>
+      <c r="N27" s="27"/>
+      <c r="O27" s="27"/>
+      <c r="P27" s="27"/>
+      <c r="Q27" s="27"/>
+      <c r="R27" s="27"/>
+      <c r="S27" s="27"/>
     </row>
     <row r="28" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="26"/>
@@ -7372,176 +7359,164 @@
       <c r="R28" s="27"/>
       <c r="S28" s="27"/>
     </row>
-    <row r="29" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="26"/>
       <c r="B29" s="44"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="52"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="67"/>
       <c r="E29" s="25"/>
       <c r="F29" s="29"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
       <c r="M29" s="29"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="27"/>
-    </row>
-    <row r="30" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="26"/>
-      <c r="B30" s="44"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="21"/>
-      <c r="O30" s="21"/>
-      <c r="P30" s="21"/>
-      <c r="Q30" s="21"/>
-      <c r="R30" s="21"/>
-      <c r="S30" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C32" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="53"/>
+      <c r="E32" s="79">
+        <f>8*2*E7</f>
+        <v>48</v>
+      </c>
+      <c r="F32" s="8" t="e">
+        <f>IF(SUM(F11:F17)&gt;0,E32-SUM(F11:F17),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G32" s="8" t="e">
+        <f>IF(SUM(G11:G17)&gt;0,E32-SUM(F11:G17),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H32" s="8" t="e">
+        <f>IF(SUM(H11:H17)&gt;0,F32-SUM(G11:H17),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I32" s="8" t="e">
+        <f>IF(SUM(I11:I17)&gt;0,E32-SUM(F11:I17),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J32" s="8" t="e">
+        <f>IF(SUM(J11:J17)&gt;0,E32-SUM(F11:J17),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K32" s="8" t="e">
+        <f>IF(SUM(K11:K17)&gt;0,E32-SUM(F11:K17),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="L32" s="8" t="e">
+        <f>IF(SUM(L11:L17)&gt;0,E32-SUM(F11:L17),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M32" s="8" t="e">
+        <f>IF(SUM(M11:M17)&gt;0,L32-SUM(M11:M17),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N32" s="8" t="e">
+        <f>IF(SUM(N11:N17)&gt;0,L32-SUM(M11:N17),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O32" s="8" t="e">
+        <f>IF(SUM(O11:O17)&gt;0,M32-SUM(N11:O17),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P32" s="8" t="e">
+        <f>IF(SUM(P11:P17)&gt;0,L32-SUM(M11:P17),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q32" s="8" t="e">
+        <f>IF(SUM(Q11:Q17)&gt;0,L32-SUM(M11:Q17),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R32" s="8" t="e">
+        <f>IF(SUM(R11:R17)&gt;0,L32-SUM(M11:R17),NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S32" s="8" t="e">
+        <f>IF(SUM(S11:S17)&gt;0,L32-SUM(M11:S17),NA())</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="33" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C33" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" s="53"/>
-      <c r="E33" s="79">
-        <f>8*2*E7</f>
-        <v>48</v>
-      </c>
-      <c r="F33" s="8" t="e">
-        <f>IF(SUM(F11:F18)&gt;0,E33-SUM(F11:F18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G33" s="8" t="e">
-        <f>IF(SUM(G11:G18)&gt;0,E33-SUM(F11:G18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H33" s="8" t="e">
-        <f>IF(SUM(H11:H18)&gt;0,F33-SUM(G11:H18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I33" s="8" t="e">
-        <f>IF(SUM(I11:I18)&gt;0,E33-SUM(F11:I18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J33" s="8" t="e">
-        <f>IF(SUM(J11:J18)&gt;0,E33-SUM(F11:J18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K33" s="8" t="e">
-        <f>IF(SUM(K11:K18)&gt;0,E33-SUM(F11:K18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L33" s="8" t="e">
-        <f>IF(SUM(L11:L18)&gt;0,E33-SUM(F11:L18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M33" s="8" t="e">
-        <f>IF(SUM(M11:M18)&gt;0,L33-SUM(M11:M18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N33" s="8" t="e">
-        <f>IF(SUM(N11:N18)&gt;0,L33-SUM(M11:N18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O33" s="8" t="e">
-        <f>IF(SUM(O11:O18)&gt;0,M33-SUM(N11:O18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P33" s="8" t="e">
-        <f>IF(SUM(P11:P18)&gt;0,L33-SUM(M11:P18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q33" s="8" t="e">
-        <f>IF(SUM(Q11:Q18)&gt;0,L33-SUM(M11:Q18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R33" s="8" t="e">
-        <f>IF(SUM(R11:R18)&gt;0,L33-SUM(M11:R18),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S33" s="8" t="e">
-        <f>IF(SUM(S11:S18)&gt;0,L33-SUM(M11:S18),NA())</f>
-        <v>#N/A</v>
+        <v>27</v>
+      </c>
+      <c r="D33" s="54"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="9">
+        <f>E32-(E32/14)</f>
+        <v>44.571428571428569</v>
+      </c>
+      <c r="G33" s="9">
+        <f>F33-(E32/14)</f>
+        <v>41.142857142857139</v>
+      </c>
+      <c r="H33" s="9">
+        <f>G33-(E32/14)</f>
+        <v>37.714285714285708</v>
+      </c>
+      <c r="I33" s="9">
+        <f>H33-(E32/14)</f>
+        <v>34.285714285714278</v>
+      </c>
+      <c r="J33" s="9">
+        <f>I33-(E32/14)</f>
+        <v>30.857142857142851</v>
+      </c>
+      <c r="K33" s="9">
+        <f>J33-(E32/14)</f>
+        <v>27.428571428571423</v>
+      </c>
+      <c r="L33" s="9">
+        <f>K33-(E32/14)</f>
+        <v>23.999999999999996</v>
+      </c>
+      <c r="M33" s="9">
+        <f>L33-(E32/14)</f>
+        <v>20.571428571428569</v>
+      </c>
+      <c r="N33" s="9">
+        <f>M33-(E32/14)</f>
+        <v>17.142857142857142</v>
+      </c>
+      <c r="O33" s="9">
+        <f>N33-(E32/14)</f>
+        <v>13.714285714285714</v>
+      </c>
+      <c r="P33" s="9">
+        <f>O33-(E32/14)</f>
+        <v>10.285714285714285</v>
+      </c>
+      <c r="Q33" s="9">
+        <f>P33-(E32/14)</f>
+        <v>6.8571428571428559</v>
+      </c>
+      <c r="R33" s="9">
+        <f>Q33-(E32/14)</f>
+        <v>3.4285714285714275</v>
+      </c>
+      <c r="S33" s="9">
+        <f>R33-(E32/14)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="C34" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="54"/>
-      <c r="E34" s="80"/>
-      <c r="F34" s="9">
-        <f>E33-(E33/14)</f>
-        <v>44.571428571428569</v>
-      </c>
-      <c r="G34" s="9">
-        <f>F34-(E33/14)</f>
-        <v>41.142857142857139</v>
-      </c>
-      <c r="H34" s="9">
-        <f>G34-(E33/14)</f>
-        <v>37.714285714285708</v>
-      </c>
-      <c r="I34" s="9">
-        <f>H34-(E33/14)</f>
-        <v>34.285714285714278</v>
-      </c>
-      <c r="J34" s="9">
-        <f>I34-(E33/14)</f>
-        <v>30.857142857142851</v>
-      </c>
-      <c r="K34" s="9">
-        <f>J34-(E33/14)</f>
-        <v>27.428571428571423</v>
-      </c>
-      <c r="L34" s="9">
-        <f>K34-(E33/14)</f>
-        <v>23.999999999999996</v>
-      </c>
-      <c r="M34" s="9">
-        <f>L34-(E33/14)</f>
-        <v>20.571428571428569</v>
-      </c>
-      <c r="N34" s="9">
-        <f>M34-(E33/14)</f>
-        <v>17.142857142857142</v>
-      </c>
-      <c r="O34" s="9">
-        <f>N34-(E33/14)</f>
-        <v>13.714285714285714</v>
-      </c>
-      <c r="P34" s="9">
-        <f>O34-(E33/14)</f>
-        <v>10.285714285714285</v>
-      </c>
-      <c r="Q34" s="9">
-        <f>P34-(E33/14)</f>
-        <v>6.8571428571428559</v>
-      </c>
-      <c r="R34" s="9">
-        <f>Q34-(E33/14)</f>
-        <v>3.4285714285714275</v>
-      </c>
-      <c r="S34" s="9">
-        <f>R34-(E33/14)</f>
-        <v>0</v>
-      </c>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
     </row>
     <row r="35" spans="3:19" x14ac:dyDescent="0.2">
       <c r="M35" s="4"/>
@@ -7624,15 +7599,6 @@
       <c r="R43" s="4"/>
       <c r="S43" s="4"/>
     </row>
-    <row r="44" spans="3:19" x14ac:dyDescent="0.2">
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
-      <c r="Q44" s="4"/>
-      <c r="R44" s="4"/>
-      <c r="S44" s="4"/>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" autoFilter="0"/>
   <autoFilter ref="A10:E10" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
@@ -7640,15 +7606,15 @@
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="E4:J4"/>
     <mergeCell ref="F8:L8"/>
-    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="E32:E33"/>
     <mergeCell ref="M8:S8"/>
   </mergeCells>
-  <conditionalFormatting sqref="F33:S33">
+  <conditionalFormatting sqref="F32:S32">
     <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="lessThan">
-      <formula>F34</formula>
+      <formula>F33</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="greaterThan">
-      <formula>F34</formula>
+      <formula>F33</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated sprint 1 hours
</commit_message>
<xml_diff>
--- a/Sprint_Planning_Document_v2_group.xlsx
+++ b/Sprint_Planning_Document_v2_group.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ctugroup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBC2DE6-424F-42BE-A9D2-B895D253A952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F9512D-5D11-46E5-BBEA-5EACC78266E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Anders Pedersen - Personal View" guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="2"/>
+    <customWorkbookView name="Sam Burke - Personal View" guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1440" windowHeight="741" activeSheetId="2"/>
     <customWorkbookView name="De La Cruz, Anthony - Personal View" guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
-    <customWorkbookView name="Sam Burke - Personal View" guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1440" windowHeight="741" activeSheetId="2"/>
-    <customWorkbookView name="Anders Pedersen - Personal View" guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="126">
   <si>
     <t>What is this?</t>
   </si>
@@ -448,6 +448,9 @@
   </si>
   <si>
     <t>Welcome Page (Create landing page)</t>
+  </si>
+  <si>
+    <t>Scrum Master, Product Owner and Developer Team</t>
   </si>
 </sst>
 </file>
@@ -1798,22 +1801,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>47.25</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46.75</c:v>
+                  <c:v>46.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.25</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.25</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.75</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39.25</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -3418,8 +3421,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}">
-      <selection activeCell="B15" sqref="B15"/>
+    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" topLeftCell="A7">
+      <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
@@ -3430,8 +3433,8 @@
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" topLeftCell="A7">
-      <selection activeCell="B12" sqref="B12"/>
+    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}">
+      <selection activeCell="B15" sqref="B15"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
@@ -5495,26 +5498,26 @@
     <row r="27" spans="1:133" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" showAutoFilter="1">
-      <selection activeCell="B7" sqref="B7"/>
+    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" showAutoFilter="1">
+      <selection activeCell="B43" sqref="B43"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{AC3AA21D-558C-42B9-AFD3-DEC2AA8F64B5}"/>
+      <autoFilter ref="B1:F1" xr:uid="{E1B2014D-F5A3-4712-B3B9-5D053B9CF086}"/>
     </customSheetView>
     <customSheetView guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" scale="150" showAutoFilter="1" topLeftCell="B36">
       <selection activeCell="C41" sqref="C41"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{7F2F6814-86B1-4863-AF2A-10461B55DF12}"/>
+      <autoFilter ref="B1:F1" xr:uid="{32F03769-743B-498A-9350-7315CEC5D4E4}"/>
     </customSheetView>
-    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" showAutoFilter="1">
-      <selection activeCell="B43" sqref="B43"/>
+    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" showAutoFilter="1">
+      <selection activeCell="B7" sqref="B7"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{FD189D20-B022-4CD5-9675-39B0E7B2D990}"/>
+      <autoFilter ref="B1:F1" xr:uid="{3A139BAC-EE75-408D-9E01-653511377D48}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -5534,8 +5537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31AAAAEB-B5F0-468C-BFDD-E9B5D3EFF0AD}">
   <dimension ref="A2:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5756,7 +5759,7 @@
         <v>83</v>
       </c>
       <c r="D11" s="61" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="E11" s="25">
         <v>1</v>
@@ -5797,7 +5800,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="29">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="G12" s="29"/>
       <c r="H12" s="29"/>
@@ -5824,7 +5827,7 @@
         <v>124</v>
       </c>
       <c r="D13" s="61" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="E13" s="25">
         <v>2</v>
@@ -5867,10 +5870,10 @@
       <c r="F14" s="29"/>
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27">
+      <c r="I14" s="27">
         <v>1</v>
       </c>
+      <c r="J14" s="27"/>
       <c r="K14" s="27"/>
       <c r="L14" s="27"/>
       <c r="M14" s="29"/>
@@ -5904,7 +5907,9 @@
       <c r="J15" s="27">
         <v>1</v>
       </c>
-      <c r="K15" s="27"/>
+      <c r="K15" s="27">
+        <v>1</v>
+      </c>
       <c r="L15" s="27"/>
       <c r="M15" s="29"/>
       <c r="N15" s="27"/>
@@ -5987,7 +5992,7 @@
         <v>90</v>
       </c>
       <c r="D18" s="61" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="E18" s="65">
         <v>2</v>
@@ -5998,8 +6003,12 @@
       <c r="I18" s="21">
         <v>1</v>
       </c>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
+      <c r="J18" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="K18" s="21">
+        <v>0.5</v>
+      </c>
       <c r="L18" s="21"/>
       <c r="M18" s="27"/>
       <c r="N18" s="21"/>
@@ -6113,7 +6122,7 @@
         <v>94</v>
       </c>
       <c r="D22" s="61" t="s">
-        <v>49</v>
+        <v>125</v>
       </c>
       <c r="E22" s="25">
         <v>2</v>
@@ -6398,7 +6407,7 @@
         <v>104</v>
       </c>
       <c r="D31" s="61" t="s">
-        <v>49</v>
+        <v>125</v>
       </c>
       <c r="E31" s="25">
         <v>1</v>
@@ -6447,27 +6456,27 @@
       </c>
       <c r="F36" s="8">
         <f>IF(SUM(F11:F31)&gt;0,E36-SUM(F11:F31),NA())</f>
-        <v>47.25</v>
+        <v>47</v>
       </c>
       <c r="G36" s="8">
         <f>IF(SUM(G11:G31)&gt;0,E36-SUM(F11:G31),NA())</f>
-        <v>46.75</v>
+        <v>46.5</v>
       </c>
       <c r="H36" s="8">
         <f>IF(SUM(H11:H31)&gt;0,F36-SUM(G11:H31),NA())</f>
-        <v>45.25</v>
+        <v>45</v>
       </c>
       <c r="I36" s="8">
         <f>IF(SUM(I11:I31)&gt;0,E36-SUM(F11:I31),NA())</f>
-        <v>43.25</v>
+        <v>42</v>
       </c>
       <c r="J36" s="8">
         <f>IF(SUM(J11:J31)&gt;0,E36-SUM(F11:J31),NA())</f>
-        <v>40.75</v>
+        <v>40</v>
       </c>
       <c r="K36" s="8">
         <f>IF(SUM(K11:K31)&gt;0,E36-SUM(F11:K31),NA())</f>
-        <v>39.25</v>
+        <v>37</v>
       </c>
       <c r="L36" s="8" t="e">
         <f>IF(SUM(L11:L31)&gt;0,E36-SUM(F11:L31),NA())</f>

</xml_diff>

<commit_message>
fixed missing names and title in cover sheet
</commit_message>
<xml_diff>
--- a/Sprint_Planning_Document_v2_group.xlsx
+++ b/Sprint_Planning_Document_v2_group.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ctugroup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F9512D-5D11-46E5-BBEA-5EACC78266E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F4D2F4-93CC-4DAF-9317-8408FD0C7CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="De La Cruz, Anthony - Personal View" guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
+    <customWorkbookView name="Sam Burke - Personal View" guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1440" windowHeight="741" activeSheetId="2"/>
     <customWorkbookView name="Anders Pedersen - Personal View" guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="2"/>
-    <customWorkbookView name="Sam Burke - Personal View" guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1440" windowHeight="741" activeSheetId="2"/>
-    <customWorkbookView name="De La Cruz, Anthony - Personal View" guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -177,9 +177,6 @@
     <t>week 2</t>
   </si>
   <si>
-    <t>CS491-2304A-01 Group 5</t>
-  </si>
-  <si>
     <t>Pizza Restaurant Online Ordering System</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
     <t>Jacob Lenz</t>
   </si>
   <si>
-    <t>Felicia Mach</t>
-  </si>
-  <si>
     <t>Welcome Page</t>
   </si>
   <si>
@@ -451,6 +445,12 @@
   </si>
   <si>
     <t>Scrum Master, Product Owner and Developer Team</t>
+  </si>
+  <si>
+    <t>Felicia Mach, Garret Thompson, Risa Luthor</t>
+  </si>
+  <si>
+    <t>CS492 Group 5</t>
   </si>
 </sst>
 </file>
@@ -3421,8 +3421,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" topLeftCell="A7">
-      <selection activeCell="B12" sqref="B12"/>
+    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}">
+      <selection activeCell="B15" sqref="B15"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
@@ -3433,8 +3433,8 @@
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}">
-      <selection activeCell="B15" sqref="B15"/>
+    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" topLeftCell="A7">
+      <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
@@ -3456,8 +3456,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:EC27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3490,7 +3490,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>34</v>
+        <v>125</v>
       </c>
       <c r="D4" s="42"/>
     </row>
@@ -3499,7 +3499,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="42"/>
     </row>
@@ -3508,7 +3508,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="42"/>
     </row>
@@ -3517,7 +3517,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="42"/>
     </row>
@@ -3526,7 +3526,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>38</v>
+        <v>124</v>
       </c>
       <c r="D8" s="42"/>
     </row>
@@ -3561,13 +3561,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="48" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="48" t="s">
-        <v>41</v>
       </c>
       <c r="E11" s="48">
         <v>1</v>
@@ -3576,7 +3576,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="48" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H11" s="57"/>
       <c r="I11" s="57"/>
@@ -3710,13 +3710,13 @@
         <v>2</v>
       </c>
       <c r="B12" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="48" t="s">
         <v>59</v>
-      </c>
-      <c r="C12" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="48" t="s">
-        <v>61</v>
       </c>
       <c r="E12" s="48">
         <v>1</v>
@@ -3725,7 +3725,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="48" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H12" s="57"/>
       <c r="I12" s="57"/>
@@ -3859,13 +3859,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="59" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="59" t="s">
         <v>69</v>
-      </c>
-      <c r="C13" s="59" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="59" t="s">
-        <v>71</v>
       </c>
       <c r="E13" s="59">
         <v>2</v>
@@ -3874,7 +3874,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="48" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H13" s="57"/>
       <c r="I13" s="57"/>
@@ -4008,13 +4008,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="48" t="s">
         <v>42</v>
-      </c>
-      <c r="C14" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="48" t="s">
-        <v>44</v>
       </c>
       <c r="E14" s="48">
         <v>1</v>
@@ -4023,7 +4023,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="48" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H14" s="57"/>
       <c r="I14" s="57"/>
@@ -4157,13 +4157,13 @@
         <v>6</v>
       </c>
       <c r="B15" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="48" t="s">
         <v>46</v>
-      </c>
-      <c r="C15" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="48" t="s">
-        <v>48</v>
       </c>
       <c r="E15" s="48">
         <v>1</v>
@@ -4172,7 +4172,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="48" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H15" s="57"/>
       <c r="I15" s="57"/>
@@ -4306,13 +4306,13 @@
         <v>7</v>
       </c>
       <c r="B16" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="48" t="s">
         <v>50</v>
-      </c>
-      <c r="C16" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="48" t="s">
-        <v>52</v>
       </c>
       <c r="E16" s="48">
         <v>1</v>
@@ -4455,13 +4455,13 @@
         <v>8</v>
       </c>
       <c r="B17" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="48" t="s">
         <v>53</v>
-      </c>
-      <c r="C17" s="58" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="48" t="s">
-        <v>55</v>
       </c>
       <c r="E17" s="48">
         <v>1</v>
@@ -4470,7 +4470,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="48" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H17" s="57"/>
       <c r="I17" s="57"/>
@@ -4604,13 +4604,13 @@
         <v>9</v>
       </c>
       <c r="B18" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="48" t="s">
         <v>56</v>
-      </c>
-      <c r="C18" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="48" t="s">
-        <v>58</v>
       </c>
       <c r="E18" s="48">
         <v>1</v>
@@ -4619,7 +4619,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="48" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H18" s="57"/>
       <c r="I18" s="57"/>
@@ -4753,13 +4753,13 @@
         <v>12</v>
       </c>
       <c r="B19" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="48" t="s">
         <v>78</v>
-      </c>
-      <c r="C19" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="48" t="s">
-        <v>80</v>
       </c>
       <c r="E19" s="48">
         <v>1</v>
@@ -4902,13 +4902,13 @@
         <v>13</v>
       </c>
       <c r="B20" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="48" t="s">
         <v>75</v>
-      </c>
-      <c r="C20" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="48" t="s">
-        <v>77</v>
       </c>
       <c r="E20" s="48">
         <v>2</v>
@@ -4917,7 +4917,7 @@
         <v>2</v>
       </c>
       <c r="G20" s="48" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H20" s="57"/>
       <c r="I20" s="57"/>
@@ -5051,13 +5051,13 @@
         <v>14</v>
       </c>
       <c r="B21" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="48" t="s">
         <v>72</v>
-      </c>
-      <c r="C21" s="48" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="48" t="s">
-        <v>74</v>
       </c>
       <c r="E21" s="48">
         <v>2</v>
@@ -5066,7 +5066,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="48" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H21" s="57"/>
       <c r="I21" s="57"/>
@@ -5200,13 +5200,13 @@
         <v>15</v>
       </c>
       <c r="B22" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="48" t="s">
         <v>63</v>
-      </c>
-      <c r="C22" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="48" t="s">
-        <v>65</v>
       </c>
       <c r="E22" s="48">
         <v>2</v>
@@ -5215,7 +5215,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="48" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H22" s="57"/>
       <c r="I22" s="57"/>
@@ -5349,13 +5349,13 @@
         <v>16</v>
       </c>
       <c r="B23" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="48" t="s">
         <v>66</v>
-      </c>
-      <c r="C23" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="48" t="s">
-        <v>68</v>
       </c>
       <c r="E23" s="48">
         <v>2</v>
@@ -5364,7 +5364,7 @@
         <v>2</v>
       </c>
       <c r="G23" s="48" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H23" s="57"/>
       <c r="I23" s="57"/>
@@ -5498,26 +5498,26 @@
     <row r="27" spans="1:133" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" showAutoFilter="1">
-      <selection activeCell="B43" sqref="B43"/>
+    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" showAutoFilter="1">
+      <selection activeCell="B7" sqref="B7"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{E1B2014D-F5A3-4712-B3B9-5D053B9CF086}"/>
+      <autoFilter ref="B1:F1" xr:uid="{CD22A87D-75CC-41D2-A7AC-B8B8568D9BEA}"/>
     </customSheetView>
     <customSheetView guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" scale="150" showAutoFilter="1" topLeftCell="B36">
       <selection activeCell="C41" sqref="C41"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{32F03769-743B-498A-9350-7315CEC5D4E4}"/>
+      <autoFilter ref="B1:F1" xr:uid="{A027366F-FE15-43C5-963F-1A6879014A4D}"/>
     </customSheetView>
-    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" showAutoFilter="1">
-      <selection activeCell="B7" sqref="B7"/>
+    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" showAutoFilter="1">
+      <selection activeCell="B43" sqref="B43"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{3A139BAC-EE75-408D-9E01-653511377D48}"/>
+      <autoFilter ref="B1:F1" xr:uid="{1D22507D-20B6-40EB-9FB3-208A038B7DBF}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -5537,7 +5537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31AAAAEB-B5F0-468C-BFDD-E9B5D3EFF0AD}">
   <dimension ref="A2:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -5576,7 +5576,7 @@
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="74"/>
       <c r="G4" s="74"/>
@@ -5750,16 +5750,16 @@
     </row>
     <row r="11" spans="1:19" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>83</v>
-      </c>
       <c r="D11" s="61" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E11" s="25">
         <v>1</v>
@@ -5791,7 +5791,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D12" s="61" t="s">
         <v>14</v>
@@ -5824,7 +5824,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D13" s="61" t="s">
         <v>14</v>
@@ -5859,10 +5859,10 @@
         <v>2</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D14" s="61" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E14" s="25">
         <v>1</v>
@@ -5892,10 +5892,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D15" s="61" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E15" s="25">
         <v>2</v>
@@ -5927,10 +5927,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D16" s="61" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E16" s="25">
         <v>1</v>
@@ -5958,10 +5958,10 @@
         <v>2</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D17" s="61" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E17" s="25">
         <v>1</v>
@@ -5989,10 +5989,10 @@
         <v>4</v>
       </c>
       <c r="C18" s="64" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D18" s="61" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E18" s="65">
         <v>2</v>
@@ -6026,10 +6026,10 @@
         <v>5</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D19" s="61" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E19" s="25">
         <v>1</v>
@@ -6051,16 +6051,16 @@
     </row>
     <row r="20" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B20" s="27">
         <v>5</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D20" s="61" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E20" s="25">
         <v>1</v>
@@ -6088,10 +6088,10 @@
         <v>5</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D21" s="61" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E21" s="25">
         <v>1</v>
@@ -6119,10 +6119,10 @@
         <v>6</v>
       </c>
       <c r="C22" s="64" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D22" s="61" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E22" s="25">
         <v>2</v>
@@ -6150,10 +6150,10 @@
         <v>6</v>
       </c>
       <c r="C23" s="64" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D23" s="61" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E23" s="25">
         <v>1</v>
@@ -6181,10 +6181,10 @@
         <v>6</v>
       </c>
       <c r="C24" s="64" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D24" s="61" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E24" s="25">
         <v>2</v>
@@ -6212,7 +6212,7 @@
         <v>7</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D25" s="61" t="s">
         <v>14</v>
@@ -6243,10 +6243,10 @@
         <v>8</v>
       </c>
       <c r="C26" s="64" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D26" s="61" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E26" s="65">
         <v>5</v>
@@ -6274,10 +6274,10 @@
         <v>9</v>
       </c>
       <c r="C27" s="64" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D27" s="61" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E27" s="65">
         <v>5</v>
@@ -6305,7 +6305,7 @@
         <v>12</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D28" s="61" t="s">
         <v>13</v>
@@ -6338,7 +6338,7 @@
         <v>12</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D29" s="61" t="s">
         <v>13</v>
@@ -6371,7 +6371,7 @@
         <v>12</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D30" s="61" t="s">
         <v>13</v>
@@ -6398,16 +6398,16 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" s="27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D31" s="61" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E31" s="25">
         <v>1</v>
@@ -6668,7 +6668,7 @@
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="74"/>
       <c r="G4" s="74"/>
@@ -6842,16 +6842,16 @@
     </row>
     <row r="11" spans="1:19" s="30" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D11" s="61" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E11" s="25">
         <v>1</v>
@@ -6879,7 +6879,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D12" s="61" t="s">
         <v>14</v>
@@ -6910,10 +6910,10 @@
         <v>13</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D13" s="61" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E13" s="25">
         <v>1.5</v>
@@ -6941,10 +6941,10 @@
         <v>14</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D14" s="61" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E14" s="25">
         <v>1</v>
@@ -6972,10 +6972,10 @@
         <v>14</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D15" s="61" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E15" s="25">
         <v>1</v>
@@ -7003,10 +7003,10 @@
         <v>15</v>
       </c>
       <c r="C16" s="64" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D16" s="61" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E16" s="25">
         <v>1</v>
@@ -7034,10 +7034,10 @@
         <v>15</v>
       </c>
       <c r="C17" s="64" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D17" s="61" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E17" s="65">
         <v>2</v>
@@ -7065,10 +7065,10 @@
         <v>15</v>
       </c>
       <c r="C18" s="64" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D18" s="61" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E18" s="65">
         <v>2</v>
@@ -7096,10 +7096,10 @@
         <v>16</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D19" s="61" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E19" s="65">
         <v>1</v>
@@ -7127,10 +7127,10 @@
         <v>16</v>
       </c>
       <c r="C20" s="64" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D20" s="61" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E20" s="65">
         <v>2</v>
@@ -7152,16 +7152,16 @@
     </row>
     <row r="21" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D21" s="61" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E21" s="25">
         <v>2</v>
@@ -7183,16 +7183,16 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D22" s="61" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E22" s="25">
         <v>2</v>
@@ -7214,16 +7214,16 @@
     </row>
     <row r="23" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A23" s="27" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D23" s="61" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E23" s="25">
         <v>1</v>
@@ -7245,16 +7245,16 @@
     </row>
     <row r="24" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A24" s="27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D24" s="61" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E24" s="25">
         <v>1</v>
@@ -7276,16 +7276,16 @@
     </row>
     <row r="25" spans="1:19" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A25" s="27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D25" s="61" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E25" s="25">
         <v>1</v>

</xml_diff>

<commit_message>
updated hours for menu design
</commit_message>
<xml_diff>
--- a/Sprint_Planning_Document_v2_group.xlsx
+++ b/Sprint_Planning_Document_v2_group.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ctugroup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F4D2F4-93CC-4DAF-9317-8408FD0C7CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56CB2AD-3E2C-4A37-87A3-65AB0005775F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Anders Pedersen - Personal View" guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="2"/>
+    <customWorkbookView name="Sam Burke - Personal View" guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1440" windowHeight="741" activeSheetId="2"/>
     <customWorkbookView name="De La Cruz, Anthony - Personal View" guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
-    <customWorkbookView name="Sam Burke - Personal View" guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1440" windowHeight="741" activeSheetId="2"/>
-    <customWorkbookView name="Anders Pedersen - Personal View" guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1819,16 +1819,16 @@
                   <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>#N/A</c:v>
+                  <c:v>36.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>#N/A</c:v>
+                  <c:v>36.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>#N/A</c:v>
+                  <c:v>35.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>#N/A</c:v>
+                  <c:v>33.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>#N/A</c:v>
@@ -3421,8 +3421,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}">
-      <selection activeCell="B15" sqref="B15"/>
+    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" topLeftCell="A7">
+      <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
@@ -3433,8 +3433,8 @@
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" topLeftCell="A7">
-      <selection activeCell="B12" sqref="B12"/>
+    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}">
+      <selection activeCell="B15" sqref="B15"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
@@ -3456,8 +3456,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:EC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5498,26 +5498,26 @@
     <row r="27" spans="1:133" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" showAutoFilter="1">
-      <selection activeCell="B7" sqref="B7"/>
+    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" showAutoFilter="1">
+      <selection activeCell="B43" sqref="B43"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{CD22A87D-75CC-41D2-A7AC-B8B8568D9BEA}"/>
+      <autoFilter ref="B1:F1" xr:uid="{025519FB-0218-42E5-8D71-3AEFDFE64D96}"/>
     </customSheetView>
     <customSheetView guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" scale="150" showAutoFilter="1" topLeftCell="B36">
       <selection activeCell="C41" sqref="C41"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{A027366F-FE15-43C5-963F-1A6879014A4D}"/>
+      <autoFilter ref="B1:F1" xr:uid="{C8AEC81E-B88F-4704-B743-B58698D41B2E}"/>
     </customSheetView>
-    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" showAutoFilter="1">
-      <selection activeCell="B43" sqref="B43"/>
+    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" showAutoFilter="1">
+      <selection activeCell="B7" sqref="B7"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{1D22507D-20B6-40EB-9FB3-208A038B7DBF}"/>
+      <autoFilter ref="B1:F1" xr:uid="{C9D54269-D8B8-4B96-90BA-85E13E10A354}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -5537,8 +5537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31AAAAEB-B5F0-468C-BFDD-E9B5D3EFF0AD}">
   <dimension ref="A2:S40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5941,7 +5941,9 @@
       <c r="I16" s="23"/>
       <c r="J16" s="23"/>
       <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
+      <c r="L16" s="23">
+        <v>0.25</v>
+      </c>
       <c r="M16" s="29"/>
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
@@ -6041,9 +6043,13 @@
       <c r="J19" s="21"/>
       <c r="K19" s="21"/>
       <c r="L19" s="21"/>
-      <c r="M19" s="27"/>
+      <c r="M19" s="27">
+        <v>0.5</v>
+      </c>
       <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
+      <c r="O19" s="21">
+        <v>0.5</v>
+      </c>
       <c r="P19" s="21"/>
       <c r="Q19" s="21"/>
       <c r="R19" s="21"/>
@@ -6074,7 +6080,9 @@
       <c r="L20" s="21"/>
       <c r="M20" s="27"/>
       <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
+      <c r="O20" s="21">
+        <v>1</v>
+      </c>
       <c r="P20" s="21"/>
       <c r="Q20" s="21"/>
       <c r="R20" s="21"/>
@@ -6104,8 +6112,12 @@
       <c r="K21" s="21"/>
       <c r="L21" s="21"/>
       <c r="M21" s="27"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="21"/>
+      <c r="N21" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="O21" s="21">
+        <v>0.5</v>
+      </c>
       <c r="P21" s="21"/>
       <c r="Q21" s="21"/>
       <c r="R21" s="21"/>
@@ -6478,21 +6490,21 @@
         <f>IF(SUM(K11:K31)&gt;0,E36-SUM(F11:K31),NA())</f>
         <v>37</v>
       </c>
-      <c r="L36" s="8" t="e">
+      <c r="L36" s="8">
         <f>IF(SUM(L11:L31)&gt;0,E36-SUM(F11:L31),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M36" s="8" t="e">
+        <v>36.75</v>
+      </c>
+      <c r="M36" s="8">
         <f>IF(SUM(M11:M31)&gt;0,L36-SUM(M11:M31),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N36" s="8" t="e">
+        <v>36.25</v>
+      </c>
+      <c r="N36" s="8">
         <f>IF(SUM(N11:N31)&gt;0,L36-SUM(M11:N31),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O36" s="8" t="e">
+        <v>35.75</v>
+      </c>
+      <c r="O36" s="8">
         <f>IF(SUM(O11:O31)&gt;0,M36-SUM(N11:O31),NA())</f>
-        <v>#N/A</v>
+        <v>33.75</v>
       </c>
       <c r="P36" s="8" t="e">
         <f>IF(SUM(P11:P31)&gt;0,L36-SUM(M11:P31),NA())</f>

</xml_diff>

<commit_message>
updated sprint 2 hours
</commit_message>
<xml_diff>
--- a/Sprint_Planning_Document_v2_group.xlsx
+++ b/Sprint_Planning_Document_v2_group.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ctugroup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5299E9A-6F14-4601-8480-CEFB9895E33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF455EE-05B7-48F7-BD33-44CB857AD7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="De La Cruz, Anthony - Personal View" guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
+    <customWorkbookView name="Sam Burke - Personal View" guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1440" windowHeight="741" activeSheetId="2"/>
     <customWorkbookView name="Anders Pedersen - Personal View" guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="2"/>
-    <customWorkbookView name="Sam Burke - Personal View" guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1440" windowHeight="741" activeSheetId="2"/>
-    <customWorkbookView name="De La Cruz, Anthony - Personal View" guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -2357,13 +2357,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>#N/A</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>#N/A</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>#N/A</c:v>
+                  <c:v>43.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -3418,8 +3418,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" topLeftCell="A7">
-      <selection activeCell="B12" sqref="B12"/>
+    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}">
+      <selection activeCell="B15" sqref="B15"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
@@ -3430,8 +3430,8 @@
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}">
-      <selection activeCell="B15" sqref="B15"/>
+    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" topLeftCell="A7">
+      <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
@@ -5495,26 +5495,26 @@
     <row r="27" spans="1:133" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" showAutoFilter="1">
-      <selection activeCell="B43" sqref="B43"/>
+    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" showAutoFilter="1">
+      <selection activeCell="B7" sqref="B7"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{C3084F40-D953-452A-8287-66B26F844AAF}"/>
+      <autoFilter ref="B1:F1" xr:uid="{0BC20C4B-67BA-406A-AADC-E0B08A6E61A5}"/>
     </customSheetView>
     <customSheetView guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" scale="150" showAutoFilter="1" topLeftCell="B36">
       <selection activeCell="C41" sqref="C41"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{BDFE75BC-F2D5-435B-B4C7-5031B5183389}"/>
+      <autoFilter ref="B1:F1" xr:uid="{99C5AABA-C558-49C6-AF68-CFA8900A6272}"/>
     </customSheetView>
-    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" showAutoFilter="1">
-      <selection activeCell="B7" sqref="B7"/>
+    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" showAutoFilter="1">
+      <selection activeCell="B43" sqref="B43"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{D9850218-C7DD-42DE-A1FD-AC66D655E342}"/>
+      <autoFilter ref="B1:F1" xr:uid="{FBD744F4-10C1-41C5-B0A0-6BD57D1C74ED}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -5535,7 +5535,7 @@
   <dimension ref="A2:S39"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6635,8 +6635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482CBEFA-189F-463E-82F1-D402C5EC0D1D}">
   <dimension ref="A2:S43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="T35" sqref="T35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7048,8 +7048,12 @@
       <c r="E17" s="65">
         <v>2</v>
       </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
+      <c r="F17" s="29">
+        <v>1</v>
+      </c>
+      <c r="G17" s="29">
+        <v>1</v>
+      </c>
       <c r="H17" s="29"/>
       <c r="I17" s="29"/>
       <c r="J17" s="27"/>
@@ -7081,7 +7085,9 @@
       </c>
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
+      <c r="H18" s="29">
+        <v>2</v>
+      </c>
       <c r="I18" s="29"/>
       <c r="J18" s="27"/>
       <c r="K18" s="27"/>
@@ -7174,7 +7180,9 @@
       </c>
       <c r="F21" s="29"/>
       <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="H21" s="21">
+        <v>0.25</v>
+      </c>
       <c r="I21" s="21"/>
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
@@ -7404,60 +7412,60 @@
         <f>8*2*E7</f>
         <v>48</v>
       </c>
-      <c r="F32" s="8" t="e">
-        <f>IF(SUM(F11:F17)&gt;0,E32-SUM(F11:F17),NA())</f>
+      <c r="F32" s="8">
+        <f>IF(SUM(F11:F29)&gt;0,E32-SUM(F11:F29),NA())</f>
+        <v>47</v>
+      </c>
+      <c r="G32" s="8">
+        <f>IF(SUM(G11:G29)&gt;0,E32-SUM(F11:G29),NA())</f>
+        <v>46</v>
+      </c>
+      <c r="H32" s="8">
+        <f>IF(SUM(H11:H29)&gt;0,F32-SUM(G11:H29),NA())</f>
+        <v>43.75</v>
+      </c>
+      <c r="I32" s="8" t="e">
+        <f>IF(SUM(I11:I29)&gt;0,E32-SUM(F11:I29),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="G32" s="8" t="e">
-        <f>IF(SUM(G11:G17)&gt;0,E32-SUM(F11:G17),NA())</f>
+      <c r="J32" s="8" t="e">
+        <f>IF(SUM(J11:J29)&gt;0,E32-SUM(F11:J29),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="H32" s="8" t="e">
-        <f>IF(SUM(H11:H17)&gt;0,F32-SUM(G11:H17),NA())</f>
+      <c r="K32" s="8" t="e">
+        <f>IF(SUM(K11:K29)&gt;0,E32-SUM(F11:K29),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="I32" s="8" t="e">
-        <f>IF(SUM(I11:I17)&gt;0,E32-SUM(F11:I17),NA())</f>
+      <c r="L32" s="8" t="e">
+        <f>IF(SUM(L11:L29)&gt;0,E32-SUM(F11:L29),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="J32" s="8" t="e">
-        <f>IF(SUM(J11:J17)&gt;0,E32-SUM(F11:J17),NA())</f>
+      <c r="M32" s="8" t="e">
+        <f>IF(SUM(M11:M29)&gt;0,L32-SUM(M11:M29),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="K32" s="8" t="e">
-        <f>IF(SUM(K11:K17)&gt;0,E32-SUM(F11:K17),NA())</f>
+      <c r="N32" s="8" t="e">
+        <f>IF(SUM(N11:N29)&gt;0,L32-SUM(M11:N29),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="L32" s="8" t="e">
-        <f>IF(SUM(L11:L17)&gt;0,E32-SUM(F11:L17),NA())</f>
+      <c r="O32" s="8" t="e">
+        <f>IF(SUM(O11:O29)&gt;0,M32-SUM(N11:O29),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="M32" s="8" t="e">
-        <f>IF(SUM(M11:M17)&gt;0,L32-SUM(M11:M17),NA())</f>
+      <c r="P32" s="8" t="e">
+        <f>IF(SUM(P11:P29)&gt;0,L32-SUM(M11:P29),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="N32" s="8" t="e">
-        <f>IF(SUM(N11:N17)&gt;0,L32-SUM(M11:N17),NA())</f>
+      <c r="Q32" s="8" t="e">
+        <f>IF(SUM(Q11:Q29)&gt;0,L32-SUM(M11:Q29),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="O32" s="8" t="e">
-        <f>IF(SUM(O11:O17)&gt;0,M32-SUM(N11:O17),NA())</f>
+      <c r="R32" s="8" t="e">
+        <f>IF(SUM(R11:R29)&gt;0,L32-SUM(M11:R29),NA())</f>
         <v>#N/A</v>
       </c>
-      <c r="P32" s="8" t="e">
-        <f>IF(SUM(P11:P17)&gt;0,L32-SUM(M11:P17),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q32" s="8" t="e">
-        <f>IF(SUM(Q11:Q17)&gt;0,L32-SUM(M11:Q17),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R32" s="8" t="e">
-        <f>IF(SUM(R11:R17)&gt;0,L32-SUM(M11:R17),NA())</f>
-        <v>#N/A</v>
-      </c>
       <c r="S32" s="8" t="e">
-        <f>IF(SUM(S11:S17)&gt;0,L32-SUM(M11:S17),NA())</f>
+        <f>IF(SUM(S11:S29)&gt;0,L32-SUM(M11:S29),NA())</f>
         <v>#N/A</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed story IDs in sprint 2
</commit_message>
<xml_diff>
--- a/Sprint_Planning_Document_v2_group.xlsx
+++ b/Sprint_Planning_Document_v2_group.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ctugroup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF455EE-05B7-48F7-BD33-44CB857AD7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DFFDE5-6658-4BDE-A4FA-5073C1297E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Anders Pedersen - Personal View" guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="2"/>
+    <customWorkbookView name="Sam Burke - Personal View" guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1440" windowHeight="741" activeSheetId="2"/>
     <customWorkbookView name="De La Cruz, Anthony - Personal View" guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
-    <customWorkbookView name="Sam Burke - Personal View" guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1440" windowHeight="741" activeSheetId="2"/>
-    <customWorkbookView name="Anders Pedersen - Personal View" guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3418,8 +3418,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}">
-      <selection activeCell="B15" sqref="B15"/>
+    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" topLeftCell="A7">
+      <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
@@ -3430,8 +3430,8 @@
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" topLeftCell="A7">
-      <selection activeCell="B12" sqref="B12"/>
+    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}">
+      <selection activeCell="B15" sqref="B15"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
@@ -5495,26 +5495,26 @@
     <row r="27" spans="1:133" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" showAutoFilter="1">
-      <selection activeCell="B7" sqref="B7"/>
+    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" showAutoFilter="1">
+      <selection activeCell="B43" sqref="B43"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{0BC20C4B-67BA-406A-AADC-E0B08A6E61A5}"/>
+      <autoFilter ref="B1:F1" xr:uid="{CF54670C-597B-4319-9B23-6A47B29F6C0D}"/>
     </customSheetView>
     <customSheetView guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" scale="150" showAutoFilter="1" topLeftCell="B36">
       <selection activeCell="C41" sqref="C41"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{99C5AABA-C558-49C6-AF68-CFA8900A6272}"/>
+      <autoFilter ref="B1:F1" xr:uid="{EBEA13DD-DAD5-4920-AA6F-5F16F275A69C}"/>
     </customSheetView>
-    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" showAutoFilter="1">
-      <selection activeCell="B43" sqref="B43"/>
+    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" showAutoFilter="1">
+      <selection activeCell="B7" sqref="B7"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{FBD744F4-10C1-41C5-B0A0-6BD57D1C74ED}"/>
+      <autoFilter ref="B1:F1" xr:uid="{688001BC-A855-4E5B-A038-B1CC227E7E11}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -6636,12 +6636,13 @@
   <dimension ref="A2:S43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="T35" sqref="T35"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="6.85546875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="5" customWidth="1"/>
     <col min="3" max="3" width="33.85546875" style="6" customWidth="1"/>
     <col min="4" max="4" width="51.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" style="4" customWidth="1"/>
@@ -6882,7 +6883,7 @@
         <v>13.1</v>
       </c>
       <c r="B12" s="27">
-        <v>13</v>
+        <v>13.1</v>
       </c>
       <c r="C12" s="28" t="s">
         <v>116</v>
@@ -6913,7 +6914,7 @@
         <v>13.2</v>
       </c>
       <c r="B13" s="27">
-        <v>13</v>
+        <v>13.2</v>
       </c>
       <c r="C13" s="28" t="s">
         <v>117</v>
@@ -6944,7 +6945,7 @@
         <v>14.2</v>
       </c>
       <c r="B14" s="44">
-        <v>14</v>
+        <v>14.1</v>
       </c>
       <c r="C14" s="28" t="s">
         <v>118</v>
@@ -6975,7 +6976,7 @@
         <v>14.3</v>
       </c>
       <c r="B15" s="44">
-        <v>14</v>
+        <v>14.2</v>
       </c>
       <c r="C15" s="28" t="s">
         <v>119</v>
@@ -7006,7 +7007,7 @@
         <v>15.1</v>
       </c>
       <c r="B16" s="27">
-        <v>15</v>
+        <v>15.1</v>
       </c>
       <c r="C16" s="64" t="s">
         <v>103</v>
@@ -7037,7 +7038,7 @@
         <v>15.2</v>
       </c>
       <c r="B17" s="27">
-        <v>15</v>
+        <v>15.2</v>
       </c>
       <c r="C17" s="64" t="s">
         <v>104</v>
@@ -7072,7 +7073,7 @@
         <v>15.3</v>
       </c>
       <c r="B18" s="27">
-        <v>15</v>
+        <v>15.3</v>
       </c>
       <c r="C18" s="64" t="s">
         <v>105</v>
@@ -7105,7 +7106,7 @@
         <v>16.100000000000001</v>
       </c>
       <c r="B19" s="63">
-        <v>16</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="C19" s="64" t="s">
         <v>106</v>
@@ -7136,7 +7137,7 @@
         <v>16.2</v>
       </c>
       <c r="B20" s="63">
-        <v>16</v>
+        <v>16.2</v>
       </c>
       <c r="C20" s="64" t="s">
         <v>107</v>

</xml_diff>

<commit_message>
updated sprint 2 week 1 hours
</commit_message>
<xml_diff>
--- a/Sprint_Planning_Document_v2_group.xlsx
+++ b/Sprint_Planning_Document_v2_group.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ctugroup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9437FD1-3E3A-4360-A413-BC4EDAD7F88A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DB0823-2FFD-4EBF-8E17-90337955BDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Anders Pedersen - Personal View" guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="2"/>
+    <customWorkbookView name="Sam Burke - Personal View" guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1440" windowHeight="741" activeSheetId="2"/>
     <customWorkbookView name="De La Cruz, Anthony - Personal View" guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
-    <customWorkbookView name="Sam Burke - Personal View" guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1440" windowHeight="741" activeSheetId="2"/>
-    <customWorkbookView name="Anders Pedersen - Personal View" guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -2366,13 +2366,13 @@
                   <c:v>38.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>#N/A</c:v>
+                  <c:v>36.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>#N/A</c:v>
+                  <c:v>34.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>#N/A</c:v>
+                  <c:v>33.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -3418,8 +3418,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}">
-      <selection activeCell="B15" sqref="B15"/>
+    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" topLeftCell="A7">
+      <selection activeCell="B12" sqref="B12"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
@@ -3430,8 +3430,8 @@
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" topLeftCell="A7">
-      <selection activeCell="B12" sqref="B12"/>
+    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}">
+      <selection activeCell="B15" sqref="B15"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
@@ -5495,26 +5495,26 @@
     <row r="27" spans="1:133" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" showAutoFilter="1">
-      <selection activeCell="B7" sqref="B7"/>
+    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" showAutoFilter="1">
+      <selection activeCell="B43" sqref="B43"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{1001BDF1-1571-4FC2-9549-79261C01F46E}"/>
+      <autoFilter ref="B1:F1" xr:uid="{86B38F1D-C7AB-4BA5-A4E3-AE73E36FC758}"/>
     </customSheetView>
     <customSheetView guid="{AF9CDD9E-3CB3-EE48-8887-F1090B6AE042}" scale="150" showAutoFilter="1" topLeftCell="B36">
       <selection activeCell="C41" sqref="C41"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{52040568-DF9E-41B0-BD07-39383EF638A0}"/>
+      <autoFilter ref="B1:F1" xr:uid="{3F0AEEE4-FBDC-4846-9A2D-A453ADF3F8B0}"/>
     </customSheetView>
-    <customSheetView guid="{988818D5-2AEF-4A9A-A55E-18240173EC63}" showAutoFilter="1">
-      <selection activeCell="B43" sqref="B43"/>
+    <customSheetView guid="{F117AA09-D9DE-4D2E-A2DF-77AB3D7617C3}" showAutoFilter="1">
+      <selection activeCell="B7" sqref="B7"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:F1" xr:uid="{4F9B849E-89F0-49BB-80CC-050454B03288}"/>
+      <autoFilter ref="B1:F1" xr:uid="{EDE85D59-0D36-4F20-B2EA-9673C1D74DBB}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">
@@ -6635,8 +6635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482CBEFA-189F-463E-82F1-D402C5EC0D1D}">
   <dimension ref="A2:S43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6900,8 +6900,12 @@
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
+      <c r="J12" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="K12" s="21">
+        <v>0.5</v>
+      </c>
       <c r="L12" s="21"/>
       <c r="M12" s="27"/>
       <c r="N12" s="21"/>
@@ -6930,7 +6934,9 @@
       <c r="F13" s="29"/>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
+      <c r="I13" s="21">
+        <v>1</v>
+      </c>
       <c r="J13" s="21"/>
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
@@ -6962,7 +6968,9 @@
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
+      <c r="J14" s="27">
+        <v>0.25</v>
+      </c>
       <c r="K14" s="27"/>
       <c r="L14" s="27"/>
       <c r="M14" s="29"/>
@@ -6992,8 +7000,12 @@
       <c r="F15" s="29"/>
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
+      <c r="I15" s="27">
+        <v>1</v>
+      </c>
+      <c r="J15" s="27">
+        <v>1</v>
+      </c>
       <c r="K15" s="27"/>
       <c r="L15" s="27"/>
       <c r="M15" s="29"/>
@@ -7128,7 +7140,9 @@
       <c r="H19" s="27"/>
       <c r="I19" s="27"/>
       <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
+      <c r="K19" s="27">
+        <v>0.5</v>
+      </c>
       <c r="L19" s="27"/>
       <c r="M19" s="29"/>
       <c r="N19" s="27"/>
@@ -7191,7 +7205,9 @@
         <v>0.25</v>
       </c>
       <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
+      <c r="J21" s="21">
+        <v>0.25</v>
+      </c>
       <c r="K21" s="21"/>
       <c r="L21" s="21"/>
       <c r="M21" s="27"/>
@@ -7224,7 +7240,9 @@
       </c>
       <c r="H22" s="21"/>
       <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
+      <c r="J22" s="21">
+        <v>0.25</v>
+      </c>
       <c r="K22" s="21"/>
       <c r="L22" s="21"/>
       <c r="M22" s="27"/>
@@ -7255,7 +7273,9 @@
       <c r="G23" s="21"/>
       <c r="H23" s="21"/>
       <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
+      <c r="J23" s="21">
+        <v>0.25</v>
+      </c>
       <c r="K23" s="21"/>
       <c r="L23" s="21"/>
       <c r="M23" s="27"/>
@@ -7433,17 +7453,17 @@
         <f>IF(SUM(H11:H29)&gt;0,F32-SUM(G11:H29),NA())</f>
         <v>38.75</v>
       </c>
-      <c r="I32" s="8" t="e">
+      <c r="I32" s="8">
         <f>IF(SUM(I11:I29)&gt;0,E32-SUM(F11:I29),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J32" s="8" t="e">
+        <v>36.75</v>
+      </c>
+      <c r="J32" s="8">
         <f>IF(SUM(J11:J29)&gt;0,E32-SUM(F11:J29),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K32" s="8" t="e">
+        <v>34.25</v>
+      </c>
+      <c r="K32" s="8">
         <f>IF(SUM(K11:K29)&gt;0,E32-SUM(F11:K29),NA())</f>
-        <v>#N/A</v>
+        <v>33.25</v>
       </c>
       <c r="L32" s="8" t="e">
         <f>IF(SUM(L11:L29)&gt;0,E32-SUM(F11:L29),NA())</f>

</xml_diff>